<commit_message>
zmiany w all tables
</commit_message>
<xml_diff>
--- a/Round5_full_hw/All_tables.xlsx
+++ b/Round5_full_hw/All_tables.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="7"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Cycle_estimation" sheetId="1" state="visible" r:id="rId2"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1595" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1626" uniqueCount="169">
   <si>
     <t xml:space="preserve">Parameter set:</t>
   </si>
@@ -441,7 +441,16 @@
     <t xml:space="preserve">Load PK</t>
   </si>
   <si>
+    <t xml:space="preserve">LoadRnd*</t>
+  </si>
+  <si>
     <t xml:space="preserve">ENC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OutCT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OutK</t>
   </si>
   <si>
     <t xml:space="preserve">Load SK</t>
@@ -483,6 +492,18 @@
     <t xml:space="preserve">XefFix</t>
   </si>
   <si>
+    <t xml:space="preserve">CCA ENCAPS:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GenL_G_R</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LoadPK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CCA DECAPS:</t>
+  </si>
+  <si>
     <t xml:space="preserve">CCA Encrypt</t>
   </si>
   <si>
@@ -505,9 +526,6 @@
   </si>
   <si>
     <t xml:space="preserve">INCLUDED IN SK!</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LoadPK</t>
   </si>
   <si>
     <t xml:space="preserve">Move</t>
@@ -857,7 +875,7 @@
   <dimension ref="A1:U75"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A11" activeCellId="1" sqref="B4:T16 A11"/>
+      <selection pane="topLeft" activeCell="A11" activeCellId="1" sqref="S90:S101 A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2334,7 +2352,7 @@
   <dimension ref="A1:J29"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B36" activeCellId="1" sqref="B4:T16 B36"/>
+      <selection pane="topLeft" activeCell="B36" activeCellId="1" sqref="S90:S101 B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3091,7 +3109,7 @@
   <dimension ref="A1:I114"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="B4:T16 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="S90:S101 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6763,7 +6781,7 @@
   <dimension ref="A1:P114"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="B4:T16 A2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="S90:S101 A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -11743,7 +11761,7 @@
   <dimension ref="A1:J39"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A24" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A24" activeCellId="1" sqref="B4:T16 A24"/>
+      <selection pane="topLeft" activeCell="A24" activeCellId="1" sqref="S90:S101 A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -13249,7 +13267,7 @@
   <dimension ref="A1:J39"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G2" activeCellId="1" sqref="B4:T16 G2"/>
+      <selection pane="topLeft" activeCell="G2" activeCellId="1" sqref="S90:S101 G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -14747,8 +14765,8 @@
   </sheetPr>
   <dimension ref="A1:X72"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="L46" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="W70" activeCellId="1" sqref="B4:T16 W70"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C25" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="W70" activeCellId="1" sqref="S90:S101 W70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -16294,10 +16312,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B6:T1048576"/>
+  <dimension ref="B6:T19"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4:T16"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="O15" activeCellId="1" sqref="S90:S101 O15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -16518,166 +16536,211 @@
         <v>137</v>
       </c>
       <c r="C11" s="24" t="n">
-        <f aca="false">C12-C10</f>
-        <v>2897</v>
+        <v>4</v>
       </c>
       <c r="D11" s="24" t="n">
-        <f aca="false">D12-D10</f>
-        <v>3740</v>
+        <v>6</v>
       </c>
       <c r="E11" s="24" t="n">
-        <f aca="false">E12-E10</f>
-        <v>4875</v>
+        <v>8</v>
       </c>
       <c r="F11" s="24" t="n">
-        <f aca="false">F12-F10</f>
-        <v>2308</v>
+        <v>4</v>
       </c>
       <c r="G11" s="24" t="n">
-        <f aca="false">G12-G10</f>
-        <v>3582</v>
+        <v>6</v>
       </c>
       <c r="H11" s="24" t="n">
-        <f aca="false">H12-H10</f>
-        <v>4435</v>
+        <v>8</v>
       </c>
       <c r="I11" s="24" t="n">
-        <f aca="false">I12-I10</f>
-        <v>2727</v>
+        <v>2</v>
       </c>
       <c r="J11" s="24" t="n">
-        <f aca="false">J12-J10</f>
-        <v>3902</v>
+        <v>3</v>
       </c>
       <c r="K11" s="24" t="n">
-        <f aca="false">K12-K10</f>
-        <v>5369</v>
+        <v>4</v>
       </c>
       <c r="L11" s="24" t="n">
-        <f aca="false">L12-L10</f>
-        <v>2360</v>
+        <v>2</v>
       </c>
       <c r="M11" s="24" t="n">
-        <f aca="false">M12-M10</f>
-        <v>3532</v>
+        <v>3</v>
       </c>
       <c r="N11" s="24" t="n">
-        <f aca="false">N12-N10</f>
-        <v>4371</v>
+        <v>4</v>
       </c>
       <c r="O11" s="24" t="n">
-        <f aca="false">O12-O10</f>
-        <v>2759</v>
+        <v>2</v>
       </c>
       <c r="P11" s="24" t="n">
-        <f aca="false">P12-P10</f>
-        <v>3941</v>
+        <v>3</v>
       </c>
       <c r="Q11" s="24" t="n">
-        <f aca="false">Q12-Q10</f>
-        <v>5413</v>
+        <v>4</v>
       </c>
       <c r="R11" s="24" t="n">
-        <f aca="false">R12-R10</f>
-        <v>2392</v>
+        <v>2</v>
       </c>
       <c r="S11" s="24" t="n">
-        <f aca="false">S12-S10</f>
-        <v>3565</v>
+        <v>3</v>
       </c>
       <c r="T11" s="24" t="n">
-        <f aca="false">T12-T10</f>
-        <v>4415</v>
+        <v>4</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="0" t="s">
-        <v>54</v>
+        <v>138</v>
       </c>
       <c r="C12" s="24" t="n">
-        <v>2977</v>
+        <f aca="false">C15-C10-C11-C13-C14</f>
+        <v>2805</v>
       </c>
       <c r="D12" s="24" t="n">
-        <v>3854</v>
+        <f aca="false">D15-D10-D11-D13-D14</f>
+        <v>3608</v>
       </c>
       <c r="E12" s="24" t="n">
-        <v>5023</v>
+        <f aca="false">E15-E10-E11-E13-E14</f>
+        <v>4701</v>
       </c>
       <c r="F12" s="24" t="n">
-        <v>2364</v>
+        <f aca="false">F15-F10-F11-F13-F14</f>
+        <v>2231</v>
       </c>
       <c r="G12" s="24" t="n">
-        <v>3680</v>
+        <f aca="false">G15-G10-G11-G13-G14</f>
+        <v>3463</v>
       </c>
       <c r="H12" s="24" t="n">
-        <v>4557</v>
+        <f aca="false">H15-H10-H11-H13-H14</f>
+        <v>4288</v>
       </c>
       <c r="I12" s="24" t="n">
-        <f aca="false">O12-32</f>
-        <v>2812</v>
+        <f aca="false">I15-I10</f>
+        <v>2727</v>
       </c>
       <c r="J12" s="24" t="n">
-        <f aca="false">P12-39</f>
-        <v>4025</v>
+        <f aca="false">J15-J10</f>
+        <v>3902</v>
       </c>
       <c r="K12" s="24" t="n">
-        <f aca="false">Q12-44</f>
-        <v>5538</v>
+        <f aca="false">K15-K10</f>
+        <v>5369</v>
       </c>
       <c r="L12" s="24" t="n">
-        <f aca="false">R12-32</f>
-        <v>2418</v>
+        <f aca="false">L15-L10</f>
+        <v>2360</v>
       </c>
       <c r="M12" s="24" t="n">
-        <f aca="false">S12-33</f>
-        <v>3630</v>
+        <f aca="false">M15-M10</f>
+        <v>3532</v>
       </c>
       <c r="N12" s="24" t="n">
-        <f aca="false">T12-44</f>
-        <v>4494</v>
+        <f aca="false">N15-N10</f>
+        <v>4371</v>
       </c>
       <c r="O12" s="24" t="n">
-        <v>2844</v>
+        <f aca="false">O15-O10</f>
+        <v>2759</v>
       </c>
       <c r="P12" s="24" t="n">
-        <v>4064</v>
+        <f aca="false">P15-P10</f>
+        <v>3941</v>
       </c>
       <c r="Q12" s="24" t="n">
-        <v>5582</v>
+        <f aca="false">Q15-Q10</f>
+        <v>5413</v>
       </c>
       <c r="R12" s="24" t="n">
-        <v>2450</v>
+        <f aca="false">R15-R10</f>
+        <v>2392</v>
       </c>
       <c r="S12" s="24" t="n">
-        <v>3663</v>
+        <f aca="false">S15-S10</f>
+        <v>3565</v>
       </c>
       <c r="T12" s="24" t="n">
-        <v>4538</v>
+        <f aca="false">T15-T10</f>
+        <v>4415</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C13" s="24"/>
-      <c r="D13" s="24"/>
-      <c r="E13" s="24"/>
-      <c r="F13" s="24"/>
-      <c r="G13" s="24"/>
-      <c r="H13" s="24"/>
-      <c r="I13" s="24"/>
-      <c r="J13" s="24"/>
-      <c r="K13" s="24"/>
-      <c r="L13" s="24"/>
-      <c r="M13" s="24"/>
-      <c r="N13" s="24"/>
-      <c r="O13" s="24"/>
-      <c r="P13" s="24"/>
-      <c r="Q13" s="24"/>
-      <c r="R13" s="24"/>
-      <c r="S13" s="24"/>
-      <c r="T13" s="24"/>
+      <c r="B13" s="0" t="s">
+        <v>139</v>
+      </c>
+      <c r="C13" s="24" t="n">
+        <v>86</v>
+      </c>
+      <c r="D13" s="24" t="n">
+        <v>123</v>
+      </c>
+      <c r="E13" s="24" t="n">
+        <v>162</v>
+      </c>
+      <c r="F13" s="24" t="n">
+        <v>71</v>
+      </c>
+      <c r="G13" s="24" t="n">
+        <v>110</v>
+      </c>
+      <c r="H13" s="24" t="n">
+        <v>135</v>
+      </c>
+      <c r="I13" s="24" t="n">
+        <f aca="false">_xlfn.CEILING.MATH(724/64)</f>
+        <v>12</v>
+      </c>
+      <c r="J13" s="24" t="n">
+        <f aca="false">_xlfn.CEILING.MATH(1079/64)</f>
+        <v>17</v>
+      </c>
+      <c r="K13" s="24" t="n">
+        <f aca="false">_xlfn.CEILING.MATH(1477/64)</f>
+        <v>24</v>
+      </c>
+      <c r="L13" s="24" t="n">
+        <f aca="false">_xlfn.CEILING.MATH(604/64)</f>
+        <v>10</v>
+      </c>
+      <c r="M13" s="24" t="n">
+        <f aca="false">_xlfn.CEILING.MATH(910/64)</f>
+        <v>15</v>
+      </c>
+      <c r="N13" s="24" t="n">
+        <f aca="false">_xlfn.CEILING.MATH(1253/64)</f>
+        <v>20</v>
+      </c>
+      <c r="O13" s="24" t="n">
+        <f aca="false">I13</f>
+        <v>12</v>
+      </c>
+      <c r="P13" s="24" t="n">
+        <f aca="false">J13</f>
+        <v>17</v>
+      </c>
+      <c r="Q13" s="24" t="n">
+        <f aca="false">K13</f>
+        <v>24</v>
+      </c>
+      <c r="R13" s="24" t="n">
+        <f aca="false">L13</f>
+        <v>10</v>
+      </c>
+      <c r="S13" s="24" t="n">
+        <f aca="false">M13</f>
+        <v>15</v>
+      </c>
+      <c r="T13" s="24" t="n">
+        <f aca="false">N13</f>
+        <v>20</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="0" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="C14" s="24" t="n">
         <v>2</v>
@@ -16698,192 +16761,322 @@
         <v>4</v>
       </c>
       <c r="I14" s="24" t="n">
-        <f aca="false">O14</f>
-        <v>89</v>
+        <v>2</v>
       </c>
       <c r="J14" s="24" t="n">
-        <f aca="false">P14</f>
-        <v>129</v>
+        <v>3</v>
       </c>
       <c r="K14" s="24" t="n">
-        <f aca="false">Q14</f>
-        <v>177</v>
+        <v>4</v>
       </c>
       <c r="L14" s="24" t="n">
-        <f aca="false">R14</f>
-        <v>62</v>
+        <v>2</v>
       </c>
       <c r="M14" s="24" t="n">
-        <f aca="false">S14</f>
-        <v>104</v>
+        <v>3</v>
       </c>
       <c r="N14" s="24" t="n">
-        <f aca="false">T14</f>
-        <v>131</v>
-      </c>
-      <c r="O14" s="24" t="n">
-        <v>89</v>
-      </c>
-      <c r="P14" s="24" t="n">
-        <v>129</v>
-      </c>
-      <c r="Q14" s="24" t="n">
-        <v>177</v>
-      </c>
-      <c r="R14" s="24" t="n">
-        <v>62</v>
-      </c>
-      <c r="S14" s="24" t="n">
-        <v>104</v>
-      </c>
-      <c r="T14" s="24" t="n">
-        <v>131</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="O14" s="24"/>
+      <c r="P14" s="24"/>
+      <c r="Q14" s="24"/>
+      <c r="R14" s="24"/>
+      <c r="S14" s="24"/>
+      <c r="T14" s="24"/>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="0" t="s">
-        <v>139</v>
+        <v>54</v>
       </c>
       <c r="C15" s="24" t="n">
-        <f aca="false">C16-C14</f>
+        <v>2977</v>
+      </c>
+      <c r="D15" s="24" t="n">
+        <v>3854</v>
+      </c>
+      <c r="E15" s="24" t="n">
+        <v>5023</v>
+      </c>
+      <c r="F15" s="24" t="n">
+        <v>2364</v>
+      </c>
+      <c r="G15" s="24" t="n">
+        <v>3680</v>
+      </c>
+      <c r="H15" s="24" t="n">
+        <v>4557</v>
+      </c>
+      <c r="I15" s="24" t="n">
+        <f aca="false">O15-32</f>
+        <v>2812</v>
+      </c>
+      <c r="J15" s="24" t="n">
+        <f aca="false">P15-39</f>
+        <v>4025</v>
+      </c>
+      <c r="K15" s="24" t="n">
+        <f aca="false">Q15-44</f>
+        <v>5538</v>
+      </c>
+      <c r="L15" s="24" t="n">
+        <f aca="false">R15-32</f>
+        <v>2418</v>
+      </c>
+      <c r="M15" s="24" t="n">
+        <f aca="false">S15-33</f>
+        <v>3630</v>
+      </c>
+      <c r="N15" s="24" t="n">
+        <f aca="false">T15-44</f>
+        <v>4494</v>
+      </c>
+      <c r="O15" s="24" t="n">
+        <v>2844</v>
+      </c>
+      <c r="P15" s="24" t="n">
+        <v>4064</v>
+      </c>
+      <c r="Q15" s="24" t="n">
+        <v>5582</v>
+      </c>
+      <c r="R15" s="24" t="n">
+        <v>2450</v>
+      </c>
+      <c r="S15" s="24" t="n">
+        <v>3663</v>
+      </c>
+      <c r="T15" s="24" t="n">
+        <v>4538</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C16" s="24"/>
+      <c r="D16" s="24"/>
+      <c r="E16" s="24"/>
+      <c r="F16" s="24"/>
+      <c r="G16" s="24"/>
+      <c r="H16" s="24"/>
+      <c r="I16" s="24"/>
+      <c r="J16" s="24"/>
+      <c r="K16" s="24"/>
+      <c r="L16" s="24"/>
+      <c r="M16" s="24"/>
+      <c r="N16" s="24"/>
+      <c r="O16" s="24"/>
+      <c r="P16" s="24"/>
+      <c r="Q16" s="24"/>
+      <c r="R16" s="24"/>
+      <c r="S16" s="24"/>
+      <c r="T16" s="24"/>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B17" s="0" t="s">
+        <v>141</v>
+      </c>
+      <c r="C17" s="24" t="n">
+        <v>2</v>
+      </c>
+      <c r="D17" s="24" t="n">
+        <v>3</v>
+      </c>
+      <c r="E17" s="24" t="n">
+        <v>4</v>
+      </c>
+      <c r="F17" s="24" t="n">
+        <v>2</v>
+      </c>
+      <c r="G17" s="24" t="n">
+        <v>3</v>
+      </c>
+      <c r="H17" s="24" t="n">
+        <v>4</v>
+      </c>
+      <c r="I17" s="24" t="n">
+        <f aca="false">O17</f>
+        <v>89</v>
+      </c>
+      <c r="J17" s="24" t="n">
+        <f aca="false">P17</f>
+        <v>129</v>
+      </c>
+      <c r="K17" s="24" t="n">
+        <f aca="false">Q17</f>
+        <v>177</v>
+      </c>
+      <c r="L17" s="24" t="n">
+        <f aca="false">R17</f>
+        <v>62</v>
+      </c>
+      <c r="M17" s="24" t="n">
+        <f aca="false">S17</f>
+        <v>104</v>
+      </c>
+      <c r="N17" s="24" t="n">
+        <f aca="false">T17</f>
+        <v>131</v>
+      </c>
+      <c r="O17" s="24" t="n">
+        <v>89</v>
+      </c>
+      <c r="P17" s="24" t="n">
+        <v>129</v>
+      </c>
+      <c r="Q17" s="24" t="n">
+        <v>177</v>
+      </c>
+      <c r="R17" s="24" t="n">
+        <v>62</v>
+      </c>
+      <c r="S17" s="24" t="n">
+        <v>104</v>
+      </c>
+      <c r="T17" s="24" t="n">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B18" s="0" t="s">
+        <v>142</v>
+      </c>
+      <c r="C18" s="24" t="n">
+        <f aca="false">C19-C17</f>
         <v>1393</v>
       </c>
-      <c r="D15" s="24" t="n">
-        <f aca="false">D16-D14</f>
+      <c r="D18" s="24" t="n">
+        <f aca="false">D19-D17</f>
         <v>1780</v>
       </c>
-      <c r="E15" s="24" t="n">
-        <f aca="false">E16-E14</f>
+      <c r="E18" s="24" t="n">
+        <f aca="false">E19-E17</f>
         <v>2295</v>
       </c>
-      <c r="F15" s="24" t="n">
-        <f aca="false">F16-F14</f>
+      <c r="F18" s="24" t="n">
+        <f aca="false">F19-F17</f>
         <v>1137</v>
       </c>
-      <c r="G15" s="24" t="n">
-        <f aca="false">G16-G14</f>
+      <c r="G18" s="24" t="n">
+        <f aca="false">G19-G17</f>
         <v>1726</v>
       </c>
-      <c r="H15" s="24" t="n">
-        <f aca="false">H16-H14</f>
+      <c r="H18" s="24" t="n">
+        <f aca="false">H19-H17</f>
         <v>2123</v>
       </c>
-      <c r="I15" s="24" t="n">
-        <f aca="false">I16-I14</f>
+      <c r="I18" s="24" t="n">
+        <f aca="false">I19-I17</f>
         <v>3873</v>
       </c>
-      <c r="J15" s="24" t="n">
-        <f aca="false">J16-J14</f>
+      <c r="J18" s="24" t="n">
+        <f aca="false">J19-J17</f>
         <v>5578</v>
       </c>
-      <c r="K15" s="24" t="n">
-        <f aca="false">K16-K14</f>
+      <c r="K18" s="24" t="n">
+        <f aca="false">K19-K17</f>
         <v>7649</v>
       </c>
-      <c r="L15" s="24" t="n">
-        <f aca="false">L16-L14</f>
+      <c r="L18" s="24" t="n">
+        <f aca="false">L19-L17</f>
         <v>3362</v>
       </c>
-      <c r="M15" s="24" t="n">
-        <f aca="false">M16-M14</f>
+      <c r="M18" s="24" t="n">
+        <f aca="false">M19-M17</f>
         <v>5004</v>
       </c>
-      <c r="N15" s="24" t="n">
-        <f aca="false">N16-N14</f>
+      <c r="N18" s="24" t="n">
+        <f aca="false">N19-N17</f>
         <v>6236</v>
       </c>
-      <c r="O15" s="24" t="n">
-        <f aca="false">O16-O14</f>
+      <c r="O18" s="24" t="n">
+        <f aca="false">O19-O17</f>
         <v>3897</v>
       </c>
-      <c r="P15" s="24" t="n">
-        <f aca="false">P16-P14</f>
+      <c r="P18" s="24" t="n">
+        <f aca="false">P19-P17</f>
         <v>5602</v>
       </c>
-      <c r="Q15" s="24" t="n">
-        <f aca="false">Q16-Q14</f>
+      <c r="Q18" s="24" t="n">
+        <f aca="false">Q19-Q17</f>
         <v>7673</v>
       </c>
-      <c r="R15" s="24" t="n">
-        <f aca="false">R16-R14</f>
+      <c r="R18" s="24" t="n">
+        <f aca="false">R19-R17</f>
         <v>3386</v>
       </c>
-      <c r="S15" s="24" t="n">
-        <f aca="false">S16-S14</f>
+      <c r="S18" s="24" t="n">
+        <f aca="false">S19-S17</f>
         <v>5028</v>
       </c>
-      <c r="T15" s="24" t="n">
-        <f aca="false">T16-T14</f>
+      <c r="T18" s="24" t="n">
+        <f aca="false">T19-T17</f>
         <v>6260</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="0" t="s">
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B19" s="0" t="s">
         <v>54</v>
       </c>
-      <c r="C16" s="24" t="n">
+      <c r="C19" s="24" t="n">
         <v>1395</v>
       </c>
-      <c r="D16" s="24" t="n">
+      <c r="D19" s="24" t="n">
         <v>1783</v>
       </c>
-      <c r="E16" s="24" t="n">
+      <c r="E19" s="24" t="n">
         <v>2299</v>
       </c>
-      <c r="F16" s="24" t="n">
+      <c r="F19" s="24" t="n">
         <v>1139</v>
       </c>
-      <c r="G16" s="24" t="n">
+      <c r="G19" s="24" t="n">
         <v>1729</v>
       </c>
-      <c r="H16" s="24" t="n">
+      <c r="H19" s="24" t="n">
         <v>2127</v>
       </c>
-      <c r="I16" s="24" t="n">
-        <f aca="false">O16-24</f>
+      <c r="I19" s="24" t="n">
+        <f aca="false">O19-24</f>
         <v>3962</v>
       </c>
-      <c r="J16" s="24" t="n">
-        <f aca="false">P16-24</f>
+      <c r="J19" s="24" t="n">
+        <f aca="false">P19-24</f>
         <v>5707</v>
       </c>
-      <c r="K16" s="24" t="n">
-        <f aca="false">Q16-24</f>
+      <c r="K19" s="24" t="n">
+        <f aca="false">Q19-24</f>
         <v>7826</v>
       </c>
-      <c r="L16" s="24" t="n">
-        <f aca="false">R16-24</f>
+      <c r="L19" s="24" t="n">
+        <f aca="false">R19-24</f>
         <v>3424</v>
       </c>
-      <c r="M16" s="24" t="n">
-        <f aca="false">S16-24</f>
+      <c r="M19" s="24" t="n">
+        <f aca="false">S19-24</f>
         <v>5108</v>
       </c>
-      <c r="N16" s="24" t="n">
-        <f aca="false">T16-24</f>
+      <c r="N19" s="24" t="n">
+        <f aca="false">T19-24</f>
         <v>6367</v>
       </c>
-      <c r="O16" s="24" t="n">
+      <c r="O19" s="24" t="n">
         <v>3986</v>
       </c>
-      <c r="P16" s="24" t="n">
+      <c r="P19" s="24" t="n">
         <v>5731</v>
       </c>
-      <c r="Q16" s="24" t="n">
+      <c r="Q19" s="24" t="n">
         <v>7850</v>
       </c>
-      <c r="R16" s="24" t="n">
+      <c r="R19" s="24" t="n">
         <v>3448</v>
       </c>
-      <c r="S16" s="24" t="n">
+      <c r="S19" s="24" t="n">
         <v>5132</v>
       </c>
-      <c r="T16" s="24" t="n">
+      <c r="T19" s="24" t="n">
         <v>6391</v>
       </c>
     </row>
-    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <mergeCells count="11">
     <mergeCell ref="C6:N6"/>
@@ -16913,10 +17106,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:T132"/>
+  <dimension ref="A1:T178"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A91" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Q91" activeCellId="1" sqref="B4:T16 Q91"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A109" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="S90" activeCellId="0" sqref="S90:S101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -18009,7 +18202,7 @@
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D33" s="0" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18033,13 +18226,13 @@
         <v>35</v>
       </c>
       <c r="G36" s="0" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="H36" s="0" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="I36" s="0" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18161,7 +18354,7 @@
         <v>20</v>
       </c>
       <c r="M39" s="0" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18210,7 +18403,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="N40" s="0" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="O40" s="0" t="s">
         <v>45</v>
@@ -18270,7 +18463,7 @@
         <v>2482</v>
       </c>
       <c r="P41" s="25" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18398,7 +18591,7 @@
         <v>48</v>
       </c>
       <c r="S43" s="26" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18909,13 +19102,13 @@
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D58" s="0" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D60" s="0" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18980,7 +19173,7 @@
         <v>1243</v>
       </c>
       <c r="I63" s="0" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19081,7 +19274,7 @@
         <v>57</v>
       </c>
       <c r="M66" s="26" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19449,1603 +19642,3051 @@
         <v>2393</v>
       </c>
     </row>
-    <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D79" s="0" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D81" s="0" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C82" s="0" t="str">
+        <f aca="false">C61</f>
+        <v>1KEM_0d</v>
+      </c>
+      <c r="D82" s="0" t="n">
+        <f aca="false">H17</f>
+        <v>2</v>
+      </c>
+      <c r="E82" s="0" t="s">
+        <v>155</v>
+      </c>
+      <c r="F82" s="0" t="s">
+        <v>156</v>
+      </c>
+      <c r="G82" s="0" t="s">
+        <v>144</v>
+      </c>
+      <c r="H82" s="0" t="s">
+        <v>145</v>
+      </c>
+      <c r="I82" s="0" t="s">
+        <v>146</v>
+      </c>
+    </row>
     <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D83" s="0" t="s">
-        <v>58</v>
+      <c r="C83" s="0" t="str">
+        <f aca="false">C62</f>
+        <v>3KEM_0d</v>
+      </c>
+      <c r="D83" s="0" t="n">
+        <f aca="false">H18</f>
+        <v>3</v>
+      </c>
+      <c r="E83" s="0" t="n">
+        <f aca="false">_xlfn.CEILING.MATH((3*J2*8)/1088)*24</f>
+        <v>24</v>
+      </c>
+      <c r="F83" s="0" t="n">
+        <f aca="false">_xlfn.CEILING.MATH(F2/8)</f>
+        <v>80</v>
+      </c>
+      <c r="G83" s="0" t="n">
+        <f aca="false">F63</f>
+        <v>0</v>
+      </c>
+      <c r="H83" s="0" t="n">
+        <f aca="false">H63</f>
+        <v>1243</v>
+      </c>
+      <c r="I83" s="0" t="str">
+        <f aca="false">I63</f>
+        <v>XefFix</v>
+      </c>
+      <c r="J83" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="K83" s="0" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C84" s="0" t="str">
+        <f aca="false">C63</f>
+        <v>5KEM_0d</v>
+      </c>
+      <c r="D84" s="0" t="n">
+        <f aca="false">H19</f>
+        <v>4</v>
+      </c>
+      <c r="E84" s="0" t="n">
+        <f aca="false">_xlfn.CEILING.MATH((3*J3*8)/1088)*24</f>
+        <v>24</v>
+      </c>
+      <c r="F84" s="0" t="n">
+        <f aca="false">_xlfn.CEILING.MATH(F3/8)</f>
+        <v>114</v>
+      </c>
+      <c r="G84" s="0" t="n">
+        <f aca="false">F64</f>
+        <v>0</v>
+      </c>
+      <c r="H84" s="0" t="n">
+        <f aca="false">H64</f>
+        <v>1579</v>
+      </c>
+      <c r="I84" s="0" t="e">
+        <f aca="false">I64</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J84" s="0" t="n">
+        <f aca="false">_xlfn.CEILING.MATH(B48*2/1088)*24</f>
+        <v>0</v>
+      </c>
+      <c r="K84" s="0" t="n">
+        <f aca="false">_xlfn.CEILING.MATH(B48*C48/64)</f>
+        <v>0</v>
+      </c>
+      <c r="L84" s="0" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C85" s="0" t="str">
+        <f aca="false">C64</f>
+        <v>1PKE_0d</v>
+      </c>
+      <c r="D85" s="0" t="n">
+        <f aca="false">H20</f>
+        <v>2</v>
+      </c>
+      <c r="E85" s="0" t="n">
+        <f aca="false">_xlfn.CEILING.MATH((3*J4*8)/1088)*24</f>
+        <v>24</v>
+      </c>
+      <c r="F85" s="0" t="n">
+        <f aca="false">_xlfn.CEILING.MATH(F4/8)</f>
+        <v>148</v>
+      </c>
+      <c r="G85" s="0" t="n">
+        <f aca="false">F65</f>
+        <v>0</v>
+      </c>
+      <c r="H85" s="0" t="n">
+        <f aca="false">H65</f>
+        <v>2043</v>
+      </c>
+      <c r="I85" s="0" t="e">
+        <f aca="false">I65</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J85" s="0" t="n">
+        <f aca="false">_xlfn.CEILING.MATH(B49*2/1088)*24</f>
+        <v>0</v>
+      </c>
+      <c r="K85" s="0" t="n">
+        <f aca="false">_xlfn.CEILING.MATH(B49*C49/64)</f>
+        <v>0</v>
+      </c>
+      <c r="L85" s="0" t="n">
+        <f aca="false">_xlfn.CEILING.MATH(B48*2/64)</f>
+        <v>0</v>
+      </c>
+      <c r="M85" s="0" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C86" s="0" t="str">
+        <f aca="false">C65</f>
+        <v>3PKE_0d</v>
+      </c>
+      <c r="D86" s="0" t="n">
+        <f aca="false">H21</f>
+        <v>3</v>
+      </c>
+      <c r="E86" s="0" t="n">
+        <f aca="false">_xlfn.CEILING.MATH((3*J5*8)/1088)*24</f>
+        <v>24</v>
+      </c>
+      <c r="F86" s="0" t="n">
+        <f aca="false">_xlfn.CEILING.MATH(F5/8)</f>
+        <v>85</v>
+      </c>
+      <c r="G86" s="0" t="n">
+        <f aca="false">F66</f>
+        <v>0</v>
+      </c>
+      <c r="H86" s="0" t="n">
+        <f aca="false">H66</f>
+        <v>1179</v>
+      </c>
+      <c r="I86" s="0" t="e">
+        <f aca="false">I66</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J86" s="0" t="n">
+        <f aca="false">_xlfn.CEILING.MATH(B50*2/1088)*24</f>
+        <v>0</v>
+      </c>
+      <c r="K86" s="0" t="n">
+        <f aca="false">_xlfn.CEILING.MATH(B50*C50/64)</f>
+        <v>0</v>
+      </c>
+      <c r="L86" s="0" t="n">
+        <f aca="false">_xlfn.CEILING.MATH(B49*2/64)</f>
+        <v>0</v>
+      </c>
+      <c r="M86" s="0" t="n">
+        <f aca="false">_xlfn.CEILING.MATH(J48*8/K48)</f>
+        <v>3</v>
+      </c>
+      <c r="N86" s="0" t="s">
+        <v>148</v>
+      </c>
+      <c r="O86" s="0" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C87" s="0" t="str">
+        <f aca="false">C66</f>
+        <v>5PKE_0d</v>
+      </c>
+      <c r="D87" s="0" t="n">
+        <f aca="false">H22</f>
+        <v>4</v>
+      </c>
+      <c r="E87" s="0" t="n">
+        <f aca="false">_xlfn.CEILING.MATH((3*J6*8)/1088)*24</f>
+        <v>24</v>
+      </c>
+      <c r="F87" s="0" t="n">
+        <f aca="false">_xlfn.CEILING.MATH(F6/8)</f>
+        <v>123</v>
+      </c>
+      <c r="G87" s="0" t="n">
+        <f aca="false">F67</f>
+        <v>0</v>
+      </c>
+      <c r="H87" s="0" t="n">
+        <f aca="false">H67</f>
+        <v>1711</v>
+      </c>
+      <c r="I87" s="0" t="e">
+        <f aca="false">I67</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J87" s="0" t="n">
+        <f aca="false">_xlfn.CEILING.MATH(B51*2/1088)*24</f>
+        <v>0</v>
+      </c>
+      <c r="K87" s="0" t="n">
+        <f aca="false">_xlfn.CEILING.MATH(B51*C51/64)</f>
+        <v>0</v>
+      </c>
+      <c r="L87" s="0" t="n">
+        <f aca="false">_xlfn.CEILING.MATH(B50*2/64)</f>
+        <v>0</v>
+      </c>
+      <c r="M87" s="0" t="n">
+        <f aca="false">_xlfn.CEILING.MATH(J49*8/K49)</f>
+        <v>3</v>
+      </c>
+      <c r="N87" s="0" t="n">
+        <f aca="false">_xlfn.CEILING.MATH(L48/64)</f>
+        <v>1</v>
+      </c>
+      <c r="O87" s="0" t="n">
+        <f aca="false">K63</f>
+        <v>0</v>
+      </c>
+      <c r="P87" s="25" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C88" s="0" t="str">
+        <f aca="false">C67</f>
+        <v>1KEM_5d</v>
+      </c>
+      <c r="D88" s="0" t="n">
+        <f aca="false">H23</f>
+        <v>2</v>
+      </c>
+      <c r="E88" s="0" t="n">
+        <f aca="false">_xlfn.CEILING.MATH((3*J7*8)/1088)*24</f>
+        <v>24</v>
+      </c>
+      <c r="F88" s="0" t="n">
+        <f aca="false">_xlfn.CEILING.MATH(F7/8)</f>
+        <v>169</v>
+      </c>
+      <c r="G88" s="0" t="n">
+        <f aca="false">F68</f>
+        <v>0</v>
+      </c>
+      <c r="H88" s="0" t="n">
+        <f aca="false">H68</f>
+        <v>2347</v>
+      </c>
+      <c r="I88" s="0" t="e">
+        <f aca="false">I68</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J88" s="0" t="n">
+        <f aca="false">_xlfn.CEILING.MATH(B52*2/1088)*24</f>
+        <v>0</v>
+      </c>
+      <c r="K88" s="0" t="n">
+        <f aca="false">_xlfn.CEILING.MATH(B52*C52/64)</f>
+        <v>0</v>
+      </c>
+      <c r="L88" s="0" t="n">
+        <f aca="false">_xlfn.CEILING.MATH(B51*2/64)</f>
+        <v>0</v>
+      </c>
+      <c r="M88" s="0" t="e">
+        <f aca="false">_xlfn.CEILING.MATH(J50*8/K50)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N88" s="0" t="n">
+        <f aca="false">_xlfn.CEILING.MATH(L49/64)</f>
+        <v>1</v>
+      </c>
+      <c r="O88" s="0" t="n">
+        <f aca="false">K64</f>
+        <v>0</v>
+      </c>
+      <c r="P88" s="0" t="n">
+        <f aca="false">_xlfn.CEILING.MATH(H48*8/64)</f>
+        <v>1</v>
+      </c>
+      <c r="Q88" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C89" s="0" t="str">
+        <f aca="false">C68</f>
+        <v>3KEM_5d</v>
+      </c>
+      <c r="D89" s="0" t="n">
+        <f aca="false">H24</f>
+        <v>3</v>
+      </c>
+      <c r="E89" s="0" t="n">
+        <f aca="false">_xlfn.CEILING.MATH((3*J8*8)/1088)*24</f>
+        <v>24</v>
+      </c>
+      <c r="F89" s="0" t="n">
+        <f aca="false">_xlfn.CEILING.MATH(F8/8)</f>
+        <v>56</v>
+      </c>
+      <c r="G89" s="0" t="n">
+        <f aca="false">F69</f>
+        <v>0</v>
+      </c>
+      <c r="H89" s="0" t="n">
+        <f aca="false">H69</f>
+        <v>987</v>
+      </c>
+      <c r="I89" s="0" t="e">
+        <f aca="false">I69</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J89" s="0" t="n">
+        <f aca="false">_xlfn.CEILING.MATH(B53*2/1088)*24</f>
+        <v>0</v>
+      </c>
+      <c r="K89" s="0" t="n">
+        <f aca="false">_xlfn.CEILING.MATH(B53*C53/64)</f>
+        <v>0</v>
+      </c>
+      <c r="L89" s="0" t="n">
+        <f aca="false">_xlfn.CEILING.MATH(B52*2/64)</f>
+        <v>0</v>
+      </c>
+      <c r="M89" s="0" t="e">
+        <f aca="false">_xlfn.CEILING.MATH(J51*8/K51)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N89" s="0" t="n">
+        <f aca="false">_xlfn.CEILING.MATH(L50/64)</f>
+        <v>1</v>
+      </c>
+      <c r="O89" s="0" t="str">
+        <f aca="false">K65</f>
+        <v>Hash</v>
+      </c>
+      <c r="P89" s="0" t="n">
+        <f aca="false">_xlfn.CEILING.MATH(H49*8/64)</f>
+        <v>0</v>
+      </c>
+      <c r="Q89" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="R89" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="S89" s="26" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C90" s="0" t="str">
+        <f aca="false">C69</f>
+        <v>5KEM_5d</v>
+      </c>
+      <c r="D90" s="0" t="n">
+        <f aca="false">H25</f>
+        <v>4</v>
+      </c>
+      <c r="E90" s="0" t="n">
+        <f aca="false">_xlfn.CEILING.MATH((3*J9*8)/1088)*24</f>
+        <v>24</v>
+      </c>
+      <c r="F90" s="0" t="n">
+        <f aca="false">_xlfn.CEILING.MATH(F9/8)</f>
+        <v>98</v>
+      </c>
+      <c r="G90" s="0" t="n">
+        <f aca="false">F70</f>
+        <v>0</v>
+      </c>
+      <c r="H90" s="0" t="n">
+        <f aca="false">H70</f>
+        <v>1519</v>
+      </c>
+      <c r="I90" s="0" t="n">
+        <f aca="false">I70</f>
+        <v>24</v>
+      </c>
+      <c r="J90" s="0" t="n">
+        <f aca="false">_xlfn.CEILING.MATH(B54*2/1088)*24</f>
+        <v>0</v>
+      </c>
+      <c r="K90" s="0" t="n">
+        <f aca="false">_xlfn.CEILING.MATH(B54*C54/64)</f>
+        <v>0</v>
+      </c>
+      <c r="L90" s="0" t="n">
+        <f aca="false">_xlfn.CEILING.MATH(B53*2/64)</f>
+        <v>0</v>
+      </c>
+      <c r="M90" s="0" t="e">
+        <f aca="false">_xlfn.CEILING.MATH(J52*8/K52)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N90" s="0" t="n">
+        <f aca="false">_xlfn.CEILING.MATH(L51/64)</f>
+        <v>0</v>
+      </c>
+      <c r="O90" s="0" t="n">
+        <f aca="false">K66</f>
+        <v>24</v>
+      </c>
+      <c r="P90" s="0" t="n">
+        <f aca="false">_xlfn.CEILING.MATH(H50*8/64)</f>
+        <v>0</v>
+      </c>
+      <c r="Q90" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="R90" s="0" t="n">
+        <f aca="false">P88+2</f>
+        <v>3</v>
+      </c>
+      <c r="S90" s="0" t="n">
+        <f aca="false">D82+E83+F83+E37+J38+K38+L39+O41+P42+Q43+R44</f>
+        <v>3129</v>
+      </c>
+    </row>
+    <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C91" s="0" t="str">
+        <f aca="false">C70</f>
+        <v>1PKE_5d</v>
+      </c>
+      <c r="D91" s="0" t="n">
+        <f aca="false">H26</f>
+        <v>2</v>
+      </c>
+      <c r="E91" s="0" t="n">
+        <f aca="false">_xlfn.CEILING.MATH((3*J10*8)/1088)*24</f>
+        <v>24</v>
+      </c>
+      <c r="F91" s="0" t="n">
+        <f aca="false">_xlfn.CEILING.MATH(F10/8)</f>
+        <v>122</v>
+      </c>
+      <c r="G91" s="0" t="n">
+        <f aca="false">F71</f>
+        <v>0</v>
+      </c>
+      <c r="H91" s="0" t="n">
+        <f aca="false">H71</f>
+        <v>1887</v>
+      </c>
+      <c r="I91" s="0" t="n">
+        <f aca="false">I71</f>
+        <v>30</v>
+      </c>
+      <c r="J91" s="0" t="n">
+        <f aca="false">_xlfn.CEILING.MATH(B55*2/1088)*24</f>
+        <v>0</v>
+      </c>
+      <c r="K91" s="0" t="n">
+        <f aca="false">_xlfn.CEILING.MATH(B55*C55/64)</f>
+        <v>0</v>
+      </c>
+      <c r="L91" s="0" t="n">
+        <f aca="false">_xlfn.CEILING.MATH(B54*2/64)</f>
+        <v>0</v>
+      </c>
+      <c r="M91" s="0" t="e">
+        <f aca="false">_xlfn.CEILING.MATH(J53*8/K53)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N91" s="0" t="n">
+        <f aca="false">_xlfn.CEILING.MATH(L52/64)</f>
+        <v>0</v>
+      </c>
+      <c r="O91" s="0" t="n">
+        <f aca="false">K67</f>
+        <v>24</v>
+      </c>
+      <c r="P91" s="0" t="n">
+        <f aca="false">_xlfn.CEILING.MATH(H51*8/64)</f>
+        <v>0</v>
+      </c>
+      <c r="Q91" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="R91" s="0" t="n">
+        <f aca="false">P89+2</f>
+        <v>2</v>
+      </c>
+      <c r="S91" s="0" t="n">
+        <f aca="false">D83+E84+F84+E38+J39+K39+L40+O42+P43+Q44+R45</f>
+        <v>4040</v>
+      </c>
+    </row>
+    <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C92" s="0" t="str">
+        <f aca="false">C71</f>
+        <v>3PKE_5d</v>
+      </c>
+      <c r="D92" s="0" t="n">
+        <f aca="false">H27</f>
+        <v>3</v>
+      </c>
+      <c r="E92" s="0" t="n">
+        <f aca="false">_xlfn.CEILING.MATH((3*J11*8)/1088)*24</f>
+        <v>24</v>
+      </c>
+      <c r="F92" s="0" t="n">
+        <f aca="false">_xlfn.CEILING.MATH(F11/8)</f>
+        <v>58</v>
+      </c>
+      <c r="G92" s="0" t="n">
+        <f aca="false">F72</f>
+        <v>0</v>
+      </c>
+      <c r="H92" s="0" t="n">
+        <f aca="false">H72</f>
+        <v>1023</v>
+      </c>
+      <c r="I92" s="0" t="n">
+        <f aca="false">I72</f>
+        <v>32</v>
+      </c>
+      <c r="J92" s="0" t="n">
+        <f aca="false">_xlfn.CEILING.MATH(B56*2/1088)*24</f>
+        <v>0</v>
+      </c>
+      <c r="K92" s="0" t="n">
+        <f aca="false">_xlfn.CEILING.MATH(B56*C56/64)</f>
+        <v>0</v>
+      </c>
+      <c r="L92" s="0" t="n">
+        <f aca="false">_xlfn.CEILING.MATH(B55*2/64)</f>
+        <v>0</v>
+      </c>
+      <c r="M92" s="0" t="e">
+        <f aca="false">_xlfn.CEILING.MATH(J54*8/K54)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N92" s="0" t="n">
+        <f aca="false">_xlfn.CEILING.MATH(L53/64)</f>
+        <v>0</v>
+      </c>
+      <c r="O92" s="0" t="n">
+        <f aca="false">K68</f>
+        <v>24</v>
+      </c>
+      <c r="P92" s="0" t="n">
+        <f aca="false">_xlfn.CEILING.MATH(H52*8/64)</f>
+        <v>0</v>
+      </c>
+      <c r="Q92" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="R92" s="0" t="n">
+        <f aca="false">P90+2</f>
+        <v>2</v>
+      </c>
+      <c r="S92" s="0" t="n">
+        <f aca="false">D84+E85+F85+E39+J40+K40+L41+O43+P44+Q45+R46</f>
+        <v>5243</v>
+      </c>
+    </row>
+    <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C93" s="0" t="str">
+        <f aca="false">C72</f>
+        <v>5PKE_5d</v>
+      </c>
+      <c r="D93" s="0" t="n">
+        <f aca="false">H28</f>
+        <v>4</v>
+      </c>
+      <c r="E93" s="0" t="n">
+        <f aca="false">_xlfn.CEILING.MATH((3*J12*8)/1088)*24</f>
+        <v>24</v>
+      </c>
+      <c r="F93" s="0" t="n">
+        <f aca="false">_xlfn.CEILING.MATH(F12/8)</f>
+        <v>98</v>
+      </c>
+      <c r="G93" s="0" t="n">
+        <f aca="false">F73</f>
+        <v>0</v>
+      </c>
+      <c r="H93" s="0" t="n">
+        <f aca="false">H73</f>
+        <v>1519</v>
+      </c>
+      <c r="I93" s="0" t="n">
+        <f aca="false">I73</f>
+        <v>24</v>
+      </c>
+      <c r="J93" s="0" t="n">
+        <f aca="false">_xlfn.CEILING.MATH(B57*2/1088)*24</f>
+        <v>0</v>
+      </c>
+      <c r="K93" s="0" t="n">
+        <f aca="false">_xlfn.CEILING.MATH(B57*C57/64)</f>
+        <v>0</v>
+      </c>
+      <c r="L93" s="0" t="n">
+        <f aca="false">_xlfn.CEILING.MATH(B56*2/64)</f>
+        <v>0</v>
+      </c>
+      <c r="M93" s="0" t="e">
+        <f aca="false">_xlfn.CEILING.MATH(J55*8/K55)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N93" s="0" t="n">
+        <f aca="false">_xlfn.CEILING.MATH(L54/64)</f>
+        <v>0</v>
+      </c>
+      <c r="O93" s="0" t="n">
+        <f aca="false">K69</f>
+        <v>24</v>
+      </c>
+      <c r="P93" s="0" t="n">
+        <f aca="false">_xlfn.CEILING.MATH(H53*8/64)</f>
+        <v>0</v>
+      </c>
+      <c r="Q93" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="R93" s="0" t="n">
+        <f aca="false">P91+2</f>
+        <v>2</v>
+      </c>
+      <c r="S93" s="0" t="n">
+        <f aca="false">D85+E86+F86+E40+J41+K41+L42+O44+P45+Q46+R47</f>
+        <v>2870</v>
+      </c>
+    </row>
+    <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E94" s="0" t="n">
+        <f aca="false">_xlfn.CEILING.MATH((3*J13*8)/1088)*24</f>
+        <v>24</v>
+      </c>
+      <c r="F94" s="0" t="n">
+        <f aca="false">_xlfn.CEILING.MATH(F13/8)</f>
+        <v>123</v>
+      </c>
+      <c r="G94" s="0" t="n">
+        <f aca="false">F74</f>
+        <v>0</v>
+      </c>
+      <c r="H94" s="0" t="n">
+        <f aca="false">H74</f>
+        <v>1899</v>
+      </c>
+      <c r="I94" s="0" t="n">
+        <f aca="false">I74</f>
+        <v>30</v>
+      </c>
+      <c r="J94" s="0" t="n">
+        <f aca="false">_xlfn.CEILING.MATH(B58*2/1088)*24</f>
+        <v>0</v>
+      </c>
+      <c r="K94" s="0" t="n">
+        <f aca="false">_xlfn.CEILING.MATH(B58*C58/64)</f>
+        <v>0</v>
+      </c>
+      <c r="L94" s="0" t="n">
+        <f aca="false">_xlfn.CEILING.MATH(B57*2/64)</f>
+        <v>0</v>
+      </c>
+      <c r="M94" s="0" t="e">
+        <f aca="false">_xlfn.CEILING.MATH(J56*8/K56)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N94" s="0" t="n">
+        <f aca="false">_xlfn.CEILING.MATH(L55/64)</f>
+        <v>0</v>
+      </c>
+      <c r="O94" s="0" t="n">
+        <f aca="false">K70</f>
+        <v>24</v>
+      </c>
+      <c r="P94" s="0" t="n">
+        <f aca="false">_xlfn.CEILING.MATH(H54*8/64)</f>
+        <v>0</v>
+      </c>
+      <c r="Q94" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="R94" s="0" t="n">
+        <f aca="false">P92+2</f>
+        <v>2</v>
+      </c>
+      <c r="S94" s="0" t="n">
+        <f aca="false">D86+E87+F87+E41+J42+K42+L43+O45+P46+Q47+R48</f>
+        <v>4069</v>
+      </c>
+    </row>
+    <row r="95" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J95" s="0" t="n">
+        <f aca="false">_xlfn.CEILING.MATH(B59*2/1088)*24</f>
+        <v>0</v>
+      </c>
+      <c r="K95" s="0" t="n">
+        <f aca="false">_xlfn.CEILING.MATH(B59*C59/64)</f>
+        <v>0</v>
+      </c>
+      <c r="L95" s="0" t="n">
+        <f aca="false">_xlfn.CEILING.MATH(B58*2/64)</f>
+        <v>0</v>
+      </c>
+      <c r="M95" s="0" t="e">
+        <f aca="false">_xlfn.CEILING.MATH(J57*8/K57)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N95" s="0" t="n">
+        <f aca="false">_xlfn.CEILING.MATH(L56/64)</f>
+        <v>0</v>
+      </c>
+      <c r="O95" s="0" t="n">
+        <f aca="false">K71</f>
+        <v>24</v>
+      </c>
+      <c r="P95" s="0" t="n">
+        <f aca="false">_xlfn.CEILING.MATH(H55*8/64)</f>
+        <v>0</v>
+      </c>
+      <c r="Q95" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="R95" s="0" t="n">
+        <f aca="false">P93+2</f>
+        <v>2</v>
+      </c>
+      <c r="S95" s="0" t="n">
+        <f aca="false">D87+E88+F88+E42+J43+K43+L44+O46+P47+Q48+R49</f>
+        <v>5596</v>
+      </c>
+    </row>
+    <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L96" s="0" t="n">
+        <f aca="false">_xlfn.CEILING.MATH(B59*2/64)</f>
+        <v>0</v>
+      </c>
+      <c r="M96" s="0" t="e">
+        <f aca="false">_xlfn.CEILING.MATH(J58*8/K58)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N96" s="0" t="n">
+        <f aca="false">_xlfn.CEILING.MATH(L57/64)</f>
+        <v>0</v>
+      </c>
+      <c r="O96" s="0" t="n">
+        <f aca="false">K72</f>
+        <v>24</v>
+      </c>
+      <c r="P96" s="0" t="n">
+        <f aca="false">_xlfn.CEILING.MATH(H56*8/64)</f>
+        <v>0</v>
+      </c>
+      <c r="Q96" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="R96" s="0" t="n">
+        <f aca="false">P94+2</f>
+        <v>2</v>
+      </c>
+      <c r="S96" s="0" t="n">
+        <f aca="false">D88+E89+F89+E43+J44+K44+L45+O47+P48+Q49+R50</f>
+        <v>2453</v>
+      </c>
+    </row>
+    <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M97" s="0" t="e">
+        <f aca="false">_xlfn.CEILING.MATH(J59*8/K59)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N97" s="0" t="n">
+        <f aca="false">_xlfn.CEILING.MATH(L58/64)</f>
+        <v>0</v>
+      </c>
+      <c r="O97" s="0" t="n">
+        <f aca="false">K73</f>
+        <v>24</v>
+      </c>
+      <c r="P97" s="0" t="n">
+        <f aca="false">_xlfn.CEILING.MATH(H57*8/64)</f>
+        <v>0</v>
+      </c>
+      <c r="Q97" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="R97" s="0" t="n">
+        <f aca="false">P95+2</f>
+        <v>2</v>
+      </c>
+      <c r="S97" s="0" t="n">
+        <f aca="false">D89+E90+F90+E44+J45+K45+L46+O48+P49+Q50+R51</f>
+        <v>3831</v>
+      </c>
+    </row>
+    <row r="98" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="N98" s="0" t="n">
+        <f aca="false">_xlfn.CEILING.MATH(L59/64)</f>
+        <v>0</v>
+      </c>
+      <c r="O98" s="0" t="n">
+        <f aca="false">K74</f>
+        <v>24</v>
+      </c>
+      <c r="P98" s="0" t="n">
+        <f aca="false">_xlfn.CEILING.MATH(H58*8/64)</f>
+        <v>0</v>
+      </c>
+      <c r="Q98" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="R98" s="0" t="n">
+        <f aca="false">P96+2</f>
+        <v>2</v>
+      </c>
+      <c r="S98" s="0" t="n">
+        <f aca="false">D90+E91+F91+E45+J46+K46+L47+O49+P50+Q51+R52</f>
+        <v>4731</v>
+      </c>
+    </row>
+    <row r="99" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="P99" s="0" t="n">
+        <f aca="false">_xlfn.CEILING.MATH(H59*8/64)</f>
+        <v>0</v>
+      </c>
+      <c r="Q99" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="R99" s="0" t="n">
+        <f aca="false">P97+2</f>
+        <v>2</v>
+      </c>
+      <c r="S99" s="0" t="n">
+        <f aca="false">D91+E92+F92+E46+J47+K47+L48+O50+P51+Q52+R53</f>
+        <v>2392</v>
+      </c>
+    </row>
+    <row r="100" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="Q100" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="R100" s="0" t="n">
+        <f aca="false">P98+2</f>
+        <v>2</v>
+      </c>
+      <c r="S100" s="0" t="n">
+        <f aca="false">D92+E93+F93+E47+J48+K48+L49+O51+P52+Q53+R54</f>
+        <v>3615</v>
+      </c>
+    </row>
+    <row r="101" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="R101" s="0" t="n">
+        <f aca="false">P99+2</f>
+        <v>2</v>
+      </c>
+      <c r="S101" s="0" t="n">
+        <f aca="false">D93+E94+F94+E48+J49+K49+L50+O52+P53+Q54+R55</f>
+        <v>4452</v>
+      </c>
+    </row>
+    <row r="102" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="103" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="104" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D104" s="0" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="105" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="106" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D106" s="0" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="107" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C107" s="0" t="str">
+        <f aca="false">C82</f>
+        <v>1KEM_0d</v>
+      </c>
+      <c r="D107" s="0" t="n">
+        <f aca="false">G63</f>
+        <v>111</v>
+      </c>
+      <c r="E107" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="F107" s="0" t="s">
+        <v>127</v>
+      </c>
+      <c r="G107" s="0" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="108" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C108" s="0" t="str">
+        <f aca="false">C83</f>
+        <v>3KEM_0d</v>
+      </c>
+      <c r="D108" s="0" t="n">
+        <f aca="false">G64</f>
+        <v>144</v>
+      </c>
+      <c r="E108" s="0" t="n">
+        <f aca="false">_xlfn.CEILING.MATH(B48*D48/1088)*24</f>
+        <v>0</v>
+      </c>
+      <c r="G108" s="0" t="n">
+        <f aca="false">_xlfn.CEILING.MATH(B48*D48/64)</f>
+        <v>0</v>
+      </c>
+      <c r="H108" s="0" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="109" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C109" s="0" t="str">
+        <f aca="false">C84</f>
+        <v>5KEM_0d</v>
+      </c>
+      <c r="D109" s="0" t="n">
+        <f aca="false">G65</f>
+        <v>83</v>
+      </c>
+      <c r="E109" s="0" t="n">
+        <f aca="false">_xlfn.CEILING.MATH(B49*D49/1088)*24</f>
+        <v>0</v>
+      </c>
+      <c r="G109" s="0" t="n">
+        <f aca="false">_xlfn.CEILING.MATH(B49*D49/64)</f>
+        <v>0</v>
+      </c>
+      <c r="H109" s="0" t="n">
+        <f aca="false">L63</f>
+        <v>0</v>
+      </c>
+      <c r="I109" s="0" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="110" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C110" s="0" t="str">
+        <f aca="false">C85</f>
+        <v>1PKE_0d</v>
+      </c>
+      <c r="D110" s="0" t="n">
+        <f aca="false">G66</f>
+        <v>120</v>
+      </c>
+      <c r="E110" s="0" t="n">
+        <f aca="false">_xlfn.CEILING.MATH(B50*D50/1088)*24</f>
+        <v>0</v>
+      </c>
+      <c r="G110" s="0" t="n">
+        <f aca="false">_xlfn.CEILING.MATH(B50*D50/64)</f>
+        <v>0</v>
+      </c>
+      <c r="H110" s="0" t="n">
+        <f aca="false">L64</f>
+        <v>0</v>
+      </c>
+      <c r="I110" s="0" t="n">
+        <f aca="false">2*(_xlfn.CEILING.MATH(J48*8/K48))</f>
+        <v>6</v>
+      </c>
+      <c r="J110" s="0" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="111" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C111" s="0" t="str">
+        <f aca="false">C86</f>
+        <v>3PKE_0d</v>
+      </c>
+      <c r="D111" s="0" t="n">
+        <f aca="false">G67</f>
+        <v>165</v>
+      </c>
+      <c r="E111" s="0" t="n">
+        <f aca="false">_xlfn.CEILING.MATH(B51*D51/1088)*24</f>
+        <v>0</v>
+      </c>
+      <c r="G111" s="0" t="n">
+        <f aca="false">_xlfn.CEILING.MATH(B51*D51/64)</f>
+        <v>0</v>
+      </c>
+      <c r="H111" s="0" t="n">
+        <f aca="false">L65</f>
+        <v>0</v>
+      </c>
+      <c r="I111" s="0" t="n">
+        <f aca="false">2*(_xlfn.CEILING.MATH(J49*8/K49))</f>
+        <v>6</v>
+      </c>
+      <c r="J111" s="0" t="n">
+        <f aca="false">F63</f>
+        <v>0</v>
+      </c>
+      <c r="K111" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="112" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C112" s="0" t="str">
+        <f aca="false">C87</f>
+        <v>5PKE_0d</v>
+      </c>
+      <c r="D112" s="0" t="n">
+        <f aca="false">G68</f>
+        <v>54</v>
+      </c>
+      <c r="E112" s="0" t="n">
+        <f aca="false">_xlfn.CEILING.MATH(B52*D52/1088)*24</f>
+        <v>0</v>
+      </c>
+      <c r="G112" s="0" t="n">
+        <f aca="false">_xlfn.CEILING.MATH(B52*D52/64)</f>
+        <v>0</v>
+      </c>
+      <c r="H112" s="0" t="str">
+        <f aca="false">L66</f>
+        <v>ReadRes</v>
+      </c>
+      <c r="I112" s="0" t="e">
+        <f aca="false">2*(_xlfn.CEILING.MATH(J50*8/K50))</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J112" s="0" t="n">
+        <f aca="false">F64</f>
+        <v>0</v>
+      </c>
+      <c r="K112" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="L112" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="M112" s="26" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="113" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C113" s="0" t="str">
+        <f aca="false">C88</f>
+        <v>1KEM_5d</v>
+      </c>
+      <c r="D113" s="0" t="n">
+        <f aca="false">G69</f>
+        <v>95</v>
+      </c>
+      <c r="E113" s="0" t="n">
+        <f aca="false">_xlfn.CEILING.MATH(B53*D53/1088)*24</f>
+        <v>0</v>
+      </c>
+      <c r="G113" s="0" t="n">
+        <f aca="false">_xlfn.CEILING.MATH(B53*D53/64)</f>
+        <v>0</v>
+      </c>
+      <c r="H113" s="0" t="n">
+        <f aca="false">L67</f>
+        <v>4</v>
+      </c>
+      <c r="I113" s="0" t="e">
+        <f aca="false">2*(_xlfn.CEILING.MATH(J51*8/K51))</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J113" s="0" t="n">
+        <f aca="false">F65</f>
+        <v>0</v>
+      </c>
+      <c r="K113" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="L113" s="0" t="n">
+        <f aca="false">F63+G63</f>
+        <v>111</v>
+      </c>
+      <c r="M113" s="0" t="n">
+        <f aca="false">L113+K112+J111+H109+E108+D107</f>
+        <v>246</v>
+      </c>
+    </row>
+    <row r="114" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C114" s="0" t="str">
+        <f aca="false">C89</f>
+        <v>3KEM_5d</v>
+      </c>
+      <c r="D114" s="0" t="n">
+        <f aca="false">G70</f>
+        <v>118</v>
+      </c>
+      <c r="E114" s="0" t="n">
+        <f aca="false">_xlfn.CEILING.MATH(B54*D54/1088)*24</f>
+        <v>0</v>
+      </c>
+      <c r="G114" s="0" t="n">
+        <f aca="false">_xlfn.CEILING.MATH(B54*D54/64)</f>
+        <v>0</v>
+      </c>
+      <c r="H114" s="0" t="n">
+        <f aca="false">L68</f>
+        <v>6</v>
+      </c>
+      <c r="I114" s="0" t="e">
+        <f aca="false">2*(_xlfn.CEILING.MATH(J52*8/K52))</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J114" s="0" t="n">
+        <f aca="false">F66</f>
+        <v>0</v>
+      </c>
+      <c r="K114" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="L114" s="0" t="n">
+        <f aca="false">F64+G64</f>
+        <v>144</v>
+      </c>
+      <c r="M114" s="0" t="n">
+        <f aca="false">L114+K113+J112+H110+E109+D108</f>
+        <v>312</v>
+      </c>
+    </row>
+    <row r="115" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C115" s="0" t="str">
+        <f aca="false">C90</f>
+        <v>5KEM_5d</v>
+      </c>
+      <c r="D115" s="0" t="n">
+        <f aca="false">G71</f>
+        <v>56</v>
+      </c>
+      <c r="E115" s="0" t="n">
+        <f aca="false">_xlfn.CEILING.MATH(B55*D55/1088)*24</f>
+        <v>0</v>
+      </c>
+      <c r="G115" s="0" t="n">
+        <f aca="false">_xlfn.CEILING.MATH(B55*D55/64)</f>
+        <v>0</v>
+      </c>
+      <c r="H115" s="0" t="n">
+        <f aca="false">L69</f>
+        <v>8</v>
+      </c>
+      <c r="I115" s="0" t="e">
+        <f aca="false">2*(_xlfn.CEILING.MATH(J53*8/K53))</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J115" s="0" t="n">
+        <f aca="false">F67</f>
+        <v>0</v>
+      </c>
+      <c r="K115" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="L115" s="0" t="n">
+        <f aca="false">F65+G65</f>
+        <v>83</v>
+      </c>
+      <c r="M115" s="0" t="n">
+        <f aca="false">L115+K114+J113+H111+E110+D109</f>
+        <v>190</v>
+      </c>
+    </row>
+    <row r="116" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C116" s="0" t="str">
+        <f aca="false">C91</f>
+        <v>1PKE_5d</v>
+      </c>
+      <c r="D116" s="0" t="n">
+        <f aca="false">G72</f>
+        <v>95</v>
+      </c>
+      <c r="E116" s="0" t="n">
+        <f aca="false">_xlfn.CEILING.MATH(B56*D56/1088)*24</f>
+        <v>0</v>
+      </c>
+      <c r="G116" s="0" t="n">
+        <f aca="false">_xlfn.CEILING.MATH(B56*D56/64)</f>
+        <v>0</v>
+      </c>
+      <c r="H116" s="0" t="n">
+        <f aca="false">L70</f>
+        <v>91</v>
+      </c>
+      <c r="I116" s="0" t="e">
+        <f aca="false">2*(_xlfn.CEILING.MATH(J54*8/K54))</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J116" s="0" t="n">
+        <f aca="false">F68</f>
+        <v>0</v>
+      </c>
+      <c r="K116" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="L116" s="0" t="n">
+        <f aca="false">F66+G66</f>
+        <v>120</v>
+      </c>
+      <c r="M116" s="0" t="e">
+        <f aca="false">L116+K115+J114+H112+E111+D110</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="117" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C117" s="0" t="str">
+        <f aca="false">C92</f>
+        <v>3PKE_5d</v>
+      </c>
+      <c r="D117" s="0" t="n">
+        <f aca="false">G73</f>
+        <v>119</v>
+      </c>
+      <c r="E117" s="0" t="n">
+        <f aca="false">_xlfn.CEILING.MATH(B57*D57/1088)*24</f>
+        <v>0</v>
+      </c>
+      <c r="G117" s="0" t="n">
+        <f aca="false">_xlfn.CEILING.MATH(B57*D57/64)</f>
+        <v>0</v>
+      </c>
+      <c r="H117" s="0" t="n">
+        <f aca="false">L71</f>
+        <v>132</v>
+      </c>
+      <c r="I117" s="0" t="e">
+        <f aca="false">2*(_xlfn.CEILING.MATH(J55*8/K55))</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J117" s="0" t="n">
+        <f aca="false">F69</f>
+        <v>0</v>
+      </c>
+      <c r="K117" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="L117" s="0" t="n">
+        <f aca="false">F67+G67</f>
+        <v>165</v>
+      </c>
+      <c r="M117" s="0" t="n">
+        <f aca="false">L117+K116+J115+H113+E112+D111</f>
+        <v>358</v>
+      </c>
+    </row>
+    <row r="118" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C118" s="0" t="str">
+        <f aca="false">C93</f>
+        <v>5PKE_5d</v>
+      </c>
+      <c r="D118" s="0" t="n">
+        <f aca="false">G74</f>
+        <v>0</v>
+      </c>
+      <c r="E118" s="0" t="e">
+        <f aca="false">_xlfn.CEILING.MATH(B58*D58/1088)*24</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="G118" s="0" t="e">
+        <f aca="false">_xlfn.CEILING.MATH(B58*D58/64)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="H118" s="0" t="n">
+        <f aca="false">L72</f>
+        <v>181</v>
+      </c>
+      <c r="I118" s="0" t="e">
+        <f aca="false">2*(_xlfn.CEILING.MATH(J56*8/K56))</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J118" s="0" t="n">
+        <f aca="false">F70</f>
+        <v>0</v>
+      </c>
+      <c r="K118" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="L118" s="0" t="n">
+        <f aca="false">F68+G68</f>
+        <v>54</v>
+      </c>
+      <c r="M118" s="0" t="n">
+        <f aca="false">L118+K117+J116+H114+E113+D112</f>
+        <v>138</v>
+      </c>
+    </row>
+    <row r="119" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E119" s="0" t="n">
+        <f aca="false">_xlfn.CEILING.MATH(B59*D59/1088)*24</f>
+        <v>0</v>
+      </c>
+      <c r="G119" s="0" t="n">
+        <f aca="false">_xlfn.CEILING.MATH(B59*D59/64)</f>
+        <v>0</v>
+      </c>
+      <c r="H119" s="0" t="n">
+        <f aca="false">L73</f>
+        <v>4</v>
+      </c>
+      <c r="I119" s="0" t="e">
+        <f aca="false">2*(_xlfn.CEILING.MATH(J57*8/K57))</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J119" s="0" t="n">
+        <f aca="false">F71</f>
+        <v>0</v>
+      </c>
+      <c r="K119" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="L119" s="0" t="n">
+        <f aca="false">F69+G69</f>
+        <v>95</v>
+      </c>
+      <c r="M119" s="0" t="e">
+        <f aca="false">L119+K118+J117+H115+E114+D113+I116</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="120" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H120" s="0" t="n">
+        <f aca="false">L74</f>
+        <v>6</v>
+      </c>
+      <c r="I120" s="0" t="e">
+        <f aca="false">2*(_xlfn.CEILING.MATH(J58*8/K58))</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J120" s="0" t="n">
+        <f aca="false">F72</f>
+        <v>0</v>
+      </c>
+      <c r="K120" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="L120" s="0" t="n">
+        <f aca="false">F70+G70</f>
+        <v>118</v>
+      </c>
+      <c r="M120" s="0" t="e">
+        <f aca="false">L120+K119+J118+H116+E115+D114+I117</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="121" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I121" s="0" t="e">
+        <f aca="false">2*(_xlfn.CEILING.MATH(J59*8/K59))</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J121" s="0" t="n">
+        <f aca="false">F73</f>
+        <v>0</v>
+      </c>
+      <c r="K121" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="L121" s="0" t="n">
+        <f aca="false">F71+G71</f>
+        <v>56</v>
+      </c>
+      <c r="M121" s="0" t="e">
+        <f aca="false">L121+K120+J119+H117+E116+D115+I118</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="122" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J122" s="0" t="n">
+        <f aca="false">F74</f>
+        <v>0</v>
+      </c>
+      <c r="K122" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="L122" s="0" t="n">
+        <f aca="false">F72+G72</f>
+        <v>95</v>
+      </c>
+      <c r="M122" s="0" t="e">
+        <f aca="false">L122+K121+J120+H118+E117+D116+I119</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="123" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K123" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="L123" s="0" t="n">
+        <f aca="false">F73+G73</f>
+        <v>119</v>
+      </c>
+      <c r="M123" s="0" t="e">
+        <f aca="false">L123+K122+J121+H119+E118+D117+I120</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="124" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L124" s="0" t="n">
+        <f aca="false">F74+G74</f>
+        <v>0</v>
+      </c>
+      <c r="M124" s="0" t="e">
+        <f aca="false">L124+K123+J122+H120+E119+D118+I121</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="125" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="126" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="127" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D127" s="0" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="128" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="129" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D129" s="0" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="130" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C130" s="0" t="str">
         <f aca="false">C61</f>
         <v>1KEM_0d</v>
       </c>
-      <c r="D84" s="0" t="n">
+      <c r="D130" s="0" t="n">
         <f aca="false">_xlfn.CEILING.MATH(F2*8/64)</f>
         <v>80</v>
       </c>
-      <c r="E84" s="0" t="s">
+      <c r="E130" s="0" t="s">
         <v>59</v>
       </c>
-      <c r="F84" s="0" t="s">
+      <c r="F130" s="0" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C85" s="0" t="str">
+    <row r="131" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C131" s="0" t="str">
         <f aca="false">C62</f>
         <v>3KEM_0d</v>
       </c>
-      <c r="D85" s="0" t="n">
+      <c r="D131" s="0" t="n">
         <f aca="false">_xlfn.CEILING.MATH(F3*8/64)</f>
         <v>114</v>
       </c>
-      <c r="E85" s="0" t="n">
-        <v>24</v>
-      </c>
-      <c r="F85" s="0" t="n">
+      <c r="E131" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="F131" s="0" t="n">
         <f aca="false">_xlfn.CEILING.MATH(B2*C2/1088)*24</f>
         <v>168</v>
       </c>
-      <c r="G85" s="0" t="s">
+      <c r="G131" s="0" t="s">
         <v>61</v>
       </c>
-      <c r="H85" s="0" t="s">
+      <c r="H131" s="0" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C86" s="0" t="str">
+    <row r="132" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C132" s="0" t="str">
         <f aca="false">C63</f>
         <v>5KEM_0d</v>
       </c>
-      <c r="D86" s="0" t="n">
+      <c r="D132" s="0" t="n">
         <f aca="false">_xlfn.CEILING.MATH(F4*8/64)</f>
         <v>148</v>
       </c>
-      <c r="E86" s="0" t="n">
-        <v>24</v>
-      </c>
-      <c r="F86" s="0" t="n">
+      <c r="E132" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="F132" s="0" t="n">
         <f aca="false">_xlfn.CEILING.MATH(B3*C3/1088)*24</f>
         <v>240</v>
       </c>
-      <c r="G86" s="0" t="n">
+      <c r="G132" s="0" t="n">
         <f aca="false">_xlfn.CEILING.MATH(B2*2/1088)*24</f>
         <v>48</v>
       </c>
-      <c r="H86" s="0" t="n">
+      <c r="H132" s="0" t="n">
         <f aca="false">_xlfn.CEILING.MATH(B2*C2/64)</f>
         <v>107</v>
       </c>
-      <c r="J86" s="0" t="s">
+      <c r="J132" s="0" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C87" s="0" t="str">
+    <row r="133" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C133" s="0" t="str">
         <f aca="false">C64</f>
         <v>1PKE_0d</v>
       </c>
-      <c r="D87" s="0" t="n">
+      <c r="D133" s="0" t="n">
         <f aca="false">_xlfn.CEILING.MATH(F5*8/64)</f>
         <v>85</v>
       </c>
-      <c r="E87" s="0" t="n">
-        <v>24</v>
-      </c>
-      <c r="F87" s="0" t="n">
+      <c r="E133" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="F133" s="0" t="n">
         <f aca="false">_xlfn.CEILING.MATH(B4*C4/1088)*24</f>
         <v>336</v>
       </c>
-      <c r="G87" s="0" t="n">
+      <c r="G133" s="0" t="n">
         <f aca="false">_xlfn.CEILING.MATH(B3*2/1088)*24</f>
         <v>48</v>
       </c>
-      <c r="H87" s="0" t="n">
+      <c r="H133" s="0" t="n">
         <f aca="false">_xlfn.CEILING.MATH(B3*C3/64)</f>
         <v>160</v>
       </c>
-      <c r="J87" s="0" t="n">
+      <c r="J133" s="0" t="n">
         <f aca="false">_xlfn.CEILING.MATH(B2*2/64)</f>
         <v>20</v>
       </c>
-      <c r="K87" s="0" t="s">
-        <v>152</v>
-      </c>
-      <c r="L87" s="0" t="s">
+      <c r="K133" s="0" t="s">
+        <v>159</v>
+      </c>
+      <c r="L133" s="0" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C88" s="0" t="str">
+    <row r="134" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C134" s="0" t="str">
         <f aca="false">C65</f>
         <v>3PKE_0d</v>
       </c>
-      <c r="D88" s="0" t="n">
+      <c r="D134" s="0" t="n">
         <f aca="false">_xlfn.CEILING.MATH(F6*8/64)</f>
         <v>123</v>
       </c>
-      <c r="E88" s="0" t="n">
-        <v>24</v>
-      </c>
-      <c r="F88" s="0" t="n">
+      <c r="E134" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="F134" s="0" t="n">
         <f aca="false">_xlfn.CEILING.MATH(B5*C5/1088)*24</f>
         <v>192</v>
       </c>
-      <c r="G88" s="0" t="n">
+      <c r="G134" s="0" t="n">
         <f aca="false">_xlfn.CEILING.MATH(B4*2/1088)*24</f>
         <v>48</v>
       </c>
-      <c r="H88" s="0" t="n">
+      <c r="H134" s="0" t="n">
         <f aca="false">_xlfn.CEILING.MATH(B4*C4/64)</f>
         <v>223</v>
       </c>
-      <c r="J88" s="0" t="n">
+      <c r="J134" s="0" t="n">
         <f aca="false">_xlfn.CEILING.MATH(B3*2/64)</f>
         <v>25</v>
       </c>
-      <c r="K88" s="0" t="e">
+      <c r="K134" s="0" t="e">
         <f aca="false">M40</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="L88" s="0" t="n">
+      <c r="L134" s="0" t="n">
         <f aca="false">K17</f>
         <v>2482</v>
       </c>
-      <c r="M88" s="0" t="s">
+      <c r="M134" s="0" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C89" s="0" t="str">
+    <row r="135" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C135" s="0" t="str">
         <f aca="false">C66</f>
         <v>5PKE_0d</v>
       </c>
-      <c r="D89" s="0" t="n">
+      <c r="D135" s="0" t="n">
         <f aca="false">_xlfn.CEILING.MATH(F7*8/64)</f>
         <v>169</v>
       </c>
-      <c r="E89" s="0" t="n">
-        <v>24</v>
-      </c>
-      <c r="F89" s="0" t="n">
+      <c r="E135" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="F135" s="0" t="n">
         <f aca="false">_xlfn.CEILING.MATH(B6*C6/1088)*24</f>
         <v>240</v>
       </c>
-      <c r="G89" s="0" t="n">
+      <c r="G135" s="0" t="n">
         <f aca="false">_xlfn.CEILING.MATH(B5*2/1088)*24</f>
         <v>48</v>
       </c>
-      <c r="H89" s="0" t="n">
+      <c r="H135" s="0" t="n">
         <f aca="false">_xlfn.CEILING.MATH(B5*C5/64)</f>
         <v>120</v>
       </c>
-      <c r="J89" s="0" t="n">
+      <c r="J135" s="0" t="n">
         <f aca="false">_xlfn.CEILING.MATH(B4*2/64)</f>
         <v>32</v>
       </c>
-      <c r="K89" s="0" t="e">
+      <c r="K135" s="0" t="e">
         <f aca="false">M41</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="L89" s="0" t="n">
+      <c r="L135" s="0" t="n">
         <f aca="false">K18</f>
         <v>3154</v>
       </c>
-      <c r="M89" s="0" t="n">
+      <c r="M135" s="0" t="n">
         <f aca="false">E17+I17</f>
         <v>8</v>
       </c>
-      <c r="P89" s="0" t="s">
+      <c r="P135" s="0" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C90" s="0" t="str">
+    <row r="136" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C136" s="0" t="str">
         <f aca="false">C67</f>
         <v>1KEM_5d</v>
       </c>
-      <c r="D90" s="0" t="n">
+      <c r="D136" s="0" t="n">
         <f aca="false">_xlfn.CEILING.MATH(F8*8/64)</f>
         <v>56</v>
       </c>
-      <c r="E90" s="0" t="n">
-        <v>24</v>
-      </c>
-      <c r="F90" s="0" t="n">
+      <c r="E136" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="F136" s="0" t="n">
         <f aca="false">_xlfn.CEILING.MATH(B7*C7/1088)*24</f>
         <v>336</v>
       </c>
-      <c r="G90" s="0" t="n">
+      <c r="G136" s="0" t="n">
         <f aca="false">_xlfn.CEILING.MATH(B6*2/1088)*24</f>
         <v>48</v>
       </c>
-      <c r="H90" s="0" t="n">
+      <c r="H136" s="0" t="n">
         <f aca="false">_xlfn.CEILING.MATH(B6*C6/64)</f>
         <v>160</v>
       </c>
-      <c r="J90" s="0" t="n">
+      <c r="J136" s="0" t="n">
         <f aca="false">_xlfn.CEILING.MATH(B5*2/64)</f>
         <v>19</v>
       </c>
-      <c r="K90" s="0" t="e">
+      <c r="K136" s="0" t="e">
         <f aca="false">M42</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="L90" s="0" t="n">
+      <c r="L136" s="0" t="n">
         <f aca="false">K19</f>
         <v>4082</v>
       </c>
-      <c r="M90" s="0" t="n">
+      <c r="M136" s="0" t="n">
         <f aca="false">E18+I18</f>
         <v>12</v>
       </c>
-      <c r="P90" s="0" t="n">
-        <v>24</v>
-      </c>
-      <c r="Q90" s="0" t="s">
+      <c r="P136" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="Q136" s="0" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C91" s="0" t="str">
+    <row r="137" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C137" s="0" t="str">
         <f aca="false">C68</f>
         <v>3KEM_5d</v>
       </c>
-      <c r="D91" s="0" t="n">
+      <c r="D137" s="0" t="n">
         <f aca="false">_xlfn.CEILING.MATH(F9*8/64)</f>
         <v>98</v>
       </c>
-      <c r="E91" s="0" t="n">
-        <v>24</v>
-      </c>
-      <c r="F91" s="0" t="n">
+      <c r="E137" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="F137" s="0" t="n">
         <f aca="false">_xlfn.CEILING.MATH(B8*C8/1088)*24</f>
         <v>120</v>
       </c>
-      <c r="G91" s="0" t="n">
+      <c r="G137" s="0" t="n">
         <f aca="false">_xlfn.CEILING.MATH(B7*2/1088)*24</f>
         <v>72</v>
       </c>
-      <c r="H91" s="0" t="n">
+      <c r="H137" s="0" t="n">
         <f aca="false">_xlfn.CEILING.MATH(B7*C7/64)</f>
         <v>238</v>
       </c>
-      <c r="J91" s="0" t="n">
+      <c r="J137" s="0" t="n">
         <f aca="false">_xlfn.CEILING.MATH(B6*2/64)</f>
         <v>27</v>
       </c>
-      <c r="K91" s="0" t="e">
+      <c r="K137" s="0" t="e">
         <f aca="false">M43</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="L91" s="0" t="n">
+      <c r="L137" s="0" t="n">
         <f aca="false">K20</f>
         <v>2354</v>
       </c>
-      <c r="M91" s="0" t="n">
+      <c r="M137" s="0" t="n">
         <f aca="false">E19+I19</f>
         <v>16</v>
       </c>
-      <c r="P91" s="0" t="n">
-        <v>24</v>
-      </c>
-      <c r="Q91" s="0" t="n">
-        <f aca="false">M89+F17</f>
+      <c r="P137" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="Q137" s="0" t="n">
+        <f aca="false">M135+F17</f>
         <v>10</v>
       </c>
-      <c r="R91" s="0" t="s">
+      <c r="R137" s="0" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C92" s="0" t="str">
+    <row r="138" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C138" s="0" t="str">
         <f aca="false">C69</f>
         <v>5KEM_5d</v>
       </c>
-      <c r="D92" s="0" t="n">
+      <c r="D138" s="0" t="n">
         <f aca="false">_xlfn.CEILING.MATH(F10*8/64)</f>
         <v>122</v>
       </c>
-      <c r="E92" s="0" t="n">
-        <v>24</v>
-      </c>
-      <c r="F92" s="0" t="n">
+      <c r="E138" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="F138" s="0" t="n">
         <f aca="false">_xlfn.CEILING.MATH(B9*C9/1088)*24</f>
         <v>216</v>
       </c>
-      <c r="G92" s="0" t="n">
+      <c r="G138" s="0" t="n">
         <f aca="false">_xlfn.CEILING.MATH(B8*2/1088)*24</f>
         <v>24</v>
       </c>
-      <c r="H92" s="0" t="n">
+      <c r="H138" s="0" t="n">
         <f aca="false">_xlfn.CEILING.MATH(B8*C8/64)</f>
         <v>77</v>
       </c>
-      <c r="J92" s="0" t="n">
+      <c r="J138" s="0" t="n">
         <f aca="false">_xlfn.CEILING.MATH(B7*2/64)</f>
         <v>37</v>
       </c>
-      <c r="K92" s="0" t="e">
+      <c r="K138" s="0" t="e">
         <f aca="false">M44</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="L92" s="0" t="n">
+      <c r="L138" s="0" t="n">
         <f aca="false">K21</f>
         <v>3418</v>
       </c>
-      <c r="M92" s="0" t="n">
+      <c r="M138" s="0" t="n">
         <f aca="false">E20+I20</f>
         <v>8</v>
       </c>
-      <c r="P92" s="0" t="n">
-        <v>24</v>
-      </c>
-      <c r="Q92" s="0" t="n">
-        <f aca="false">M90+F18</f>
+      <c r="P138" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="Q138" s="0" t="n">
+        <f aca="false">M136+F18</f>
         <v>15</v>
       </c>
-      <c r="R92" s="0" t="n">
-        <v>24</v>
-      </c>
-      <c r="S92" s="0" t="s">
+      <c r="R138" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="S138" s="0" t="s">
         <v>65</v>
       </c>
-      <c r="T92" s="26" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C93" s="0" t="str">
+      <c r="T138" s="26" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="139" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C139" s="0" t="str">
         <f aca="false">C70</f>
         <v>1PKE_5d</v>
       </c>
-      <c r="D93" s="0" t="n">
+      <c r="D139" s="0" t="n">
         <f aca="false">_xlfn.CEILING.MATH(F11*8/64)</f>
         <v>58</v>
       </c>
-      <c r="E93" s="0" t="n">
-        <v>24</v>
-      </c>
-      <c r="F93" s="0" t="n">
+      <c r="E139" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="F139" s="0" t="n">
         <f aca="false">_xlfn.CEILING.MATH(B10*C10/1088)*24</f>
         <v>264</v>
       </c>
-      <c r="G93" s="0" t="n">
+      <c r="G139" s="0" t="n">
         <f aca="false">_xlfn.CEILING.MATH(B9*2/1088)*24</f>
         <v>48</v>
       </c>
-      <c r="H93" s="0" t="n">
+      <c r="H139" s="0" t="n">
         <f aca="false">_xlfn.CEILING.MATH(B9*C9/64)</f>
         <v>142</v>
       </c>
-      <c r="J93" s="0" t="n">
+      <c r="J139" s="0" t="n">
         <f aca="false">_xlfn.CEILING.MATH(B8*2/64)</f>
         <v>16</v>
       </c>
-      <c r="K93" s="0" t="e">
+      <c r="K139" s="0" t="e">
         <f aca="false">M45</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="L93" s="0" t="n">
+      <c r="L139" s="0" t="n">
         <f aca="false">K22</f>
         <v>4690</v>
       </c>
-      <c r="M93" s="0" t="n">
+      <c r="M139" s="0" t="n">
         <f aca="false">E21+I21</f>
         <v>15</v>
       </c>
-      <c r="P93" s="0" t="n">
-        <v>24</v>
-      </c>
-      <c r="Q93" s="0" t="n">
-        <f aca="false">M91+F19</f>
+      <c r="P139" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="Q139" s="0" t="n">
+        <f aca="false">M137+F19</f>
         <v>20</v>
       </c>
-      <c r="R93" s="0" t="n">
-        <v>24</v>
-      </c>
-      <c r="S93" s="0" t="n">
+      <c r="R139" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="S139" s="0" t="n">
         <f aca="false">E17</f>
         <v>8</v>
       </c>
-      <c r="T93" s="0" t="n">
-        <f aca="false">S93+R92+Q91+P90+M89+L88+J87+H86+F85+D84</f>
+      <c r="T139" s="0" t="n">
+        <f aca="false">S139+R138+Q137+P136+M135+L134+J133+H132+F131+D130</f>
         <v>2931</v>
       </c>
     </row>
-    <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C94" s="0" t="str">
+    <row r="140" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C140" s="0" t="str">
         <f aca="false">C71</f>
         <v>3PKE_5d</v>
       </c>
-      <c r="D94" s="0" t="n">
+      <c r="D140" s="0" t="n">
         <f aca="false">_xlfn.CEILING.MATH(F12*8/64)</f>
         <v>98</v>
       </c>
-      <c r="E94" s="0" t="n">
-        <v>24</v>
-      </c>
-      <c r="F94" s="0" t="n">
+      <c r="E140" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="F140" s="0" t="n">
         <f aca="false">_xlfn.CEILING.MATH(B11*C11/1088)*24</f>
         <v>120</v>
       </c>
-      <c r="G94" s="0" t="n">
+      <c r="G140" s="0" t="n">
         <f aca="false">_xlfn.CEILING.MATH(B10*2/1088)*24</f>
         <v>48</v>
       </c>
-      <c r="H94" s="0" t="n">
+      <c r="H140" s="0" t="n">
         <f aca="false">_xlfn.CEILING.MATH(B10*C10/64)</f>
         <v>177</v>
       </c>
-      <c r="J94" s="0" t="n">
+      <c r="J140" s="0" t="n">
         <f aca="false">_xlfn.CEILING.MATH(B9*2/64)</f>
         <v>24</v>
       </c>
-      <c r="K94" s="0" t="n">
+      <c r="K140" s="0" t="n">
         <f aca="false">M46</f>
         <v>12</v>
       </c>
-      <c r="L94" s="0" t="n">
+      <c r="L140" s="0" t="n">
         <f aca="false">K23</f>
         <v>1970</v>
       </c>
-      <c r="M94" s="0" t="n">
+      <c r="M140" s="0" t="n">
         <f aca="false">E22+I22</f>
         <v>20</v>
       </c>
-      <c r="P94" s="0" t="n">
-        <v>24</v>
-      </c>
-      <c r="Q94" s="0" t="n">
-        <f aca="false">M92+F20</f>
+      <c r="P140" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="Q140" s="0" t="n">
+        <f aca="false">M138+F20</f>
         <v>10</v>
       </c>
-      <c r="R94" s="0" t="n">
-        <v>24</v>
-      </c>
-      <c r="S94" s="0" t="n">
+      <c r="R140" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="S140" s="0" t="n">
         <f aca="false">E18</f>
         <v>12</v>
       </c>
-      <c r="T94" s="0" t="n">
-        <f aca="false">S94+R93+Q92+P91+M90+L89+J88+H87+F86+D85</f>
+      <c r="T140" s="0" t="n">
+        <f aca="false">S140+R139+Q138+P137+M136+L135+J134+H133+F132+D131</f>
         <v>3780</v>
       </c>
     </row>
-    <row r="95" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C95" s="0" t="str">
+    <row r="141" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C141" s="0" t="str">
         <f aca="false">C72</f>
         <v>5PKE_5d</v>
       </c>
-      <c r="D95" s="0" t="n">
+      <c r="D141" s="0" t="n">
         <f aca="false">_xlfn.CEILING.MATH(F13*8/64)</f>
         <v>123</v>
       </c>
-      <c r="E95" s="0" t="n">
-        <v>24</v>
-      </c>
-      <c r="F95" s="0" t="n">
+      <c r="E141" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="F141" s="0" t="n">
         <f aca="false">_xlfn.CEILING.MATH(B12*C12/1088)*24</f>
         <v>216</v>
       </c>
-      <c r="G95" s="0" t="n">
+      <c r="G141" s="0" t="n">
         <f aca="false">_xlfn.CEILING.MATH(B11*2/1088)*24</f>
         <v>24</v>
       </c>
-      <c r="H95" s="0" t="n">
+      <c r="H141" s="0" t="n">
         <f aca="false">_xlfn.CEILING.MATH(B11*C11/64)</f>
         <v>80</v>
       </c>
-      <c r="J95" s="0" t="n">
+      <c r="J141" s="0" t="n">
         <f aca="false">_xlfn.CEILING.MATH(B10*2/64)</f>
         <v>30</v>
       </c>
-      <c r="K95" s="0" t="n">
+      <c r="K141" s="0" t="n">
         <f aca="false">M47</f>
         <v>15</v>
       </c>
-      <c r="L95" s="0" t="n">
+      <c r="L141" s="0" t="n">
         <f aca="false">K24</f>
         <v>3034</v>
       </c>
-      <c r="M95" s="0" t="n">
+      <c r="M141" s="0" t="n">
         <f aca="false">E23+I23</f>
         <v>30</v>
       </c>
-      <c r="P95" s="0" t="n">
-        <v>24</v>
-      </c>
-      <c r="Q95" s="0" t="n">
-        <f aca="false">M93+F21</f>
+      <c r="P141" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="Q141" s="0" t="n">
+        <f aca="false">M139+F21</f>
         <v>18</v>
       </c>
-      <c r="R95" s="0" t="n">
-        <v>24</v>
-      </c>
-      <c r="S95" s="0" t="n">
+      <c r="R141" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="S141" s="0" t="n">
         <f aca="false">E19</f>
         <v>16</v>
       </c>
-      <c r="T95" s="0" t="n">
-        <f aca="false">S95+R94+Q93+P92+M91+L90+J89+H88+F87+D86</f>
+      <c r="T141" s="0" t="n">
+        <f aca="false">S141+R140+Q139+P138+M137+L136+J135+H134+F133+D132</f>
         <v>4921</v>
       </c>
     </row>
-    <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E96" s="0" t="n">
-        <v>24</v>
-      </c>
-      <c r="F96" s="0" t="n">
+    <row r="142" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E142" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="F142" s="0" t="n">
         <f aca="false">_xlfn.CEILING.MATH(B13*C13/1088)*24</f>
         <v>240</v>
       </c>
-      <c r="G96" s="0" t="n">
+      <c r="G142" s="0" t="n">
         <f aca="false">_xlfn.CEILING.MATH(B12*2/1088)*24</f>
         <v>48</v>
       </c>
-      <c r="H96" s="0" t="n">
+      <c r="H142" s="0" t="n">
         <f aca="false">_xlfn.CEILING.MATH(B12*C12/64)</f>
         <v>142</v>
       </c>
-      <c r="J96" s="0" t="n">
+      <c r="J142" s="0" t="n">
         <f aca="false">_xlfn.CEILING.MATH(B11*2/64)</f>
         <v>16</v>
       </c>
-      <c r="K96" s="0" t="n">
+      <c r="K142" s="0" t="n">
         <f aca="false">M48</f>
         <v>16</v>
       </c>
-      <c r="L96" s="0" t="n">
+      <c r="L142" s="0" t="n">
         <f aca="false">K25</f>
         <v>3770</v>
       </c>
-      <c r="M96" s="0" t="n">
+      <c r="M142" s="0" t="n">
         <f aca="false">E24+I24</f>
         <v>34</v>
       </c>
-      <c r="P96" s="0" t="n">
-        <v>24</v>
-      </c>
-      <c r="Q96" s="0" t="n">
-        <f aca="false">M94+F22</f>
-        <v>24</v>
-      </c>
-      <c r="R96" s="0" t="n">
-        <v>24</v>
-      </c>
-      <c r="S96" s="0" t="n">
+      <c r="P142" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="Q142" s="0" t="n">
+        <f aca="false">M140+F22</f>
+        <v>24</v>
+      </c>
+      <c r="R142" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="S142" s="0" t="n">
         <f aca="false">E20</f>
         <v>8</v>
       </c>
-      <c r="T96" s="0" t="n">
-        <f aca="false">S96+R95+Q94+P93+M92+L91+J90+H89+F88+D87</f>
+      <c r="T142" s="0" t="n">
+        <f aca="false">S142+R141+Q140+P139+M138+L137+J136+H135+F134+D133</f>
         <v>2844</v>
       </c>
     </row>
-    <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G97" s="0" t="n">
+    <row r="143" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G143" s="0" t="n">
         <f aca="false">_xlfn.CEILING.MATH(B13*2/1088)*24</f>
         <v>48</v>
       </c>
-      <c r="H97" s="0" t="n">
+      <c r="H143" s="0" t="n">
         <f aca="false">_xlfn.CEILING.MATH(B13*C13/64)</f>
         <v>163</v>
       </c>
-      <c r="J97" s="0" t="n">
+      <c r="J143" s="0" t="n">
         <f aca="false">_xlfn.CEILING.MATH(B12*2/64)</f>
         <v>24</v>
       </c>
-      <c r="K97" s="0" t="n">
+      <c r="K143" s="0" t="n">
         <f aca="false">M49</f>
         <v>12</v>
       </c>
-      <c r="L97" s="0" t="n">
+      <c r="L143" s="0" t="n">
         <f aca="false">K26</f>
         <v>2042</v>
       </c>
-      <c r="M97" s="0" t="n">
+      <c r="M143" s="0" t="n">
         <f aca="false">E25+I25</f>
         <v>38</v>
       </c>
-      <c r="P97" s="0" t="n">
-        <v>24</v>
-      </c>
-      <c r="Q97" s="0" t="n">
-        <f aca="false">M95+F23</f>
+      <c r="P143" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="Q143" s="0" t="n">
+        <f aca="false">M141+F23</f>
         <v>32</v>
       </c>
-      <c r="R97" s="0" t="n">
-        <v>24</v>
-      </c>
-      <c r="S97" s="0" t="n">
+      <c r="R143" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="S143" s="0" t="n">
         <f aca="false">E21</f>
         <v>15</v>
       </c>
-      <c r="T97" s="0" t="n">
-        <f aca="false">S97+R96+Q95+P94+M93+L92+J91+H90+F89+D88</f>
+      <c r="T143" s="0" t="n">
+        <f aca="false">S143+R142+Q141+P140+M139+L138+J137+H136+F135+D134</f>
         <v>4064</v>
       </c>
     </row>
-    <row r="98" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J98" s="0" t="n">
+    <row r="144" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J144" s="0" t="n">
         <f aca="false">_xlfn.CEILING.MATH(B13*2/64)</f>
         <v>30</v>
       </c>
-      <c r="K98" s="0" t="n">
+      <c r="K144" s="0" t="n">
         <f aca="false">M50</f>
         <v>15</v>
       </c>
-      <c r="L98" s="0" t="n">
+      <c r="L144" s="0" t="n">
         <f aca="false">K27</f>
         <v>3034</v>
       </c>
-      <c r="M98" s="0" t="n">
+      <c r="M144" s="0" t="n">
         <f aca="false">E26+I26</f>
         <v>32</v>
       </c>
-      <c r="P98" s="0" t="n">
-        <v>24</v>
-      </c>
-      <c r="Q98" s="0" t="n">
-        <f aca="false">M96+F24</f>
+      <c r="P144" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="Q144" s="0" t="n">
+        <f aca="false">M142+F24</f>
         <v>37</v>
       </c>
-      <c r="R98" s="0" t="n">
-        <v>24</v>
-      </c>
-      <c r="S98" s="0" t="n">
+      <c r="R144" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="S144" s="0" t="n">
         <f aca="false">E22</f>
         <v>20</v>
       </c>
-      <c r="T98" s="0" t="n">
-        <f aca="false">S98+R97+Q96+P95+M94+L93+J92+H91+F90+D89</f>
+      <c r="T144" s="0" t="n">
+        <f aca="false">S144+R143+Q142+P141+M140+L139+J138+H137+F136+D135</f>
         <v>5582</v>
       </c>
     </row>
-    <row r="99" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K99" s="0" t="n">
+    <row r="145" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K145" s="0" t="n">
         <f aca="false">M51</f>
         <v>16</v>
       </c>
-      <c r="L99" s="0" t="n">
+      <c r="L145" s="0" t="n">
         <f aca="false">K28</f>
         <v>3794</v>
       </c>
-      <c r="M99" s="0" t="n">
+      <c r="M145" s="0" t="n">
         <f aca="false">E27+I27</f>
         <v>37</v>
       </c>
-      <c r="P99" s="0" t="n">
-        <v>24</v>
-      </c>
-      <c r="Q99" s="0" t="n">
-        <f aca="false">M97+F25</f>
+      <c r="P145" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="Q145" s="0" t="n">
+        <f aca="false">M143+F25</f>
         <v>42</v>
       </c>
-      <c r="R99" s="0" t="n">
-        <v>24</v>
-      </c>
-      <c r="S99" s="0" t="n">
+      <c r="R145" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="S145" s="0" t="n">
         <f aca="false">E23</f>
         <v>6</v>
       </c>
-      <c r="T99" s="0" t="n">
-        <f aca="false">S99+R98+Q97+P96+M95+L94+J93+H92+F91+D90+K94</f>
+      <c r="T145" s="0" t="n">
+        <f aca="false">S145+R144+Q143+P142+M141+L140+J139+H138+F137+D136+K140</f>
         <v>2367</v>
       </c>
     </row>
-    <row r="100" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="M100" s="0" t="n">
+    <row r="146" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M146" s="0" t="n">
         <f aca="false">E28+I28</f>
         <v>50</v>
       </c>
-      <c r="P100" s="0" t="n">
-        <v>24</v>
-      </c>
-      <c r="Q100" s="0" t="n">
-        <f aca="false">M98+F26</f>
+      <c r="P146" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="Q146" s="0" t="n">
+        <f aca="false">M144+F26</f>
         <v>34</v>
       </c>
-      <c r="R100" s="0" t="n">
-        <v>24</v>
-      </c>
-      <c r="S100" s="0" t="n">
+      <c r="R146" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="S146" s="0" t="n">
         <f aca="false">E24</f>
         <v>6</v>
       </c>
-      <c r="T100" s="0" t="n">
-        <f aca="false">S100+R99+Q98+P97+M96+L95+J94+H93+F92+D91+K95</f>
+      <c r="T146" s="0" t="n">
+        <f aca="false">S146+R145+Q144+P143+M142+L141+J140+H139+F138+D137+K141</f>
         <v>3654</v>
       </c>
     </row>
-    <row r="101" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="P101" s="0" t="n">
-        <v>24</v>
-      </c>
-      <c r="Q101" s="0" t="n">
-        <f aca="false">M99+F27</f>
+    <row r="147" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="P147" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="Q147" s="0" t="n">
+        <f aca="false">M145+F27</f>
         <v>40</v>
       </c>
-      <c r="R101" s="0" t="n">
-        <v>24</v>
-      </c>
-      <c r="S101" s="0" t="n">
+      <c r="R147" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="S147" s="0" t="n">
         <f aca="false">E25</f>
         <v>8</v>
       </c>
-      <c r="T101" s="0" t="n">
-        <f aca="false">S101+R100+Q99+P98+M97+L96+J95+H94+F93+D92+K96</f>
+      <c r="T147" s="0" t="n">
+        <f aca="false">S147+R146+Q145+P144+M143+L142+J141+H140+F139+D138+K142</f>
         <v>4515</v>
       </c>
     </row>
-    <row r="102" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Q102" s="0" t="n">
-        <f aca="false">M100+F28</f>
+    <row r="148" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="Q148" s="0" t="n">
+        <f aca="false">M146+F28</f>
         <v>54</v>
       </c>
-      <c r="R102" s="0" t="n">
-        <v>24</v>
-      </c>
-      <c r="S102" s="0" t="n">
+      <c r="R148" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="S148" s="0" t="n">
         <f aca="false">E26</f>
         <v>8</v>
       </c>
-      <c r="T102" s="0" t="n">
-        <f aca="false">S102+R101+Q100+P99+M98+L97+J96+H95+F94+D93+K97</f>
+      <c r="T148" s="0" t="n">
+        <f aca="false">S148+R147+Q146+P145+M144+L143+J142+H141+F140+D139+K143</f>
         <v>2450</v>
       </c>
     </row>
-    <row r="103" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="R103" s="0" t="n">
-        <v>24</v>
-      </c>
-      <c r="S103" s="0" t="n">
+    <row r="149" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="R149" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="S149" s="0" t="n">
         <f aca="false">E27</f>
         <v>9</v>
       </c>
-      <c r="T103" s="0" t="n">
-        <f aca="false">S103+R102+Q101+P100+M99+L98+J97+H96+F95+D94+K98</f>
+      <c r="T149" s="0" t="n">
+        <f aca="false">S149+R148+Q147+P146+M145+L144+J143+H142+F141+D140+K144</f>
         <v>3663</v>
       </c>
     </row>
-    <row r="104" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S104" s="0" t="n">
+    <row r="150" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="S150" s="0" t="n">
         <f aca="false">E28</f>
         <v>20</v>
       </c>
-      <c r="T104" s="0" t="n">
-        <f aca="false">S104+R103+Q102+P101+M100+L99+J98+H97+F96+D95+K99</f>
+      <c r="T150" s="0" t="n">
+        <f aca="false">S150+R149+Q148+P147+M146+L145+J144+H143+F142+D141+K145</f>
         <v>4538</v>
       </c>
     </row>
-    <row r="105" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D107" s="0" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D109" s="0" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="110" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C110" s="0" t="str">
-        <f aca="false">C84</f>
+    <row r="151" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="152" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="153" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D153" s="0" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="154" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="155" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D155" s="0" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="156" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C156" s="0" t="str">
+        <f aca="false">C130</f>
         <v>1KEM_0d</v>
       </c>
-      <c r="D110" s="0" t="n">
+      <c r="D156" s="0" t="n">
         <f aca="false">_xlfn.CEILING.MATH(G2*8/64)</f>
         <v>2</v>
       </c>
-      <c r="E110" s="0" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="111" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C111" s="0" t="str">
-        <f aca="false">C85</f>
+      <c r="E156" s="0" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="157" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C157" s="0" t="str">
+        <f aca="false">C131</f>
         <v>3KEM_0d</v>
       </c>
-      <c r="D111" s="0" t="n">
+      <c r="D157" s="0" t="n">
         <f aca="false">_xlfn.CEILING.MATH(G3*8/64)</f>
         <v>3</v>
       </c>
-      <c r="E111" s="0" t="n">
+      <c r="E157" s="0" t="n">
         <f aca="false">_xlfn.CEILING.MATH(I2*8/64)</f>
         <v>2</v>
       </c>
-      <c r="F111" s="0" t="s">
+      <c r="F157" s="0" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="112" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C112" s="0" t="str">
-        <f aca="false">C86</f>
+    <row r="158" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C158" s="0" t="str">
+        <f aca="false">C132</f>
         <v>5KEM_0d</v>
       </c>
-      <c r="D112" s="0" t="n">
+      <c r="D158" s="0" t="n">
         <f aca="false">_xlfn.CEILING.MATH(G4*8/64)</f>
         <v>4</v>
       </c>
-      <c r="E112" s="0" t="n">
+      <c r="E158" s="0" t="n">
         <f aca="false">_xlfn.CEILING.MATH(I3*8/64)</f>
         <v>3</v>
       </c>
-      <c r="F112" s="0" t="n">
+      <c r="F158" s="0" t="n">
         <f aca="false">L17</f>
         <v>1243</v>
       </c>
-      <c r="G112" s="0" t="s">
-        <v>156</v>
-      </c>
-      <c r="H112" s="0" t="s">
-        <v>157</v>
-      </c>
-      <c r="J112" s="27" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="113" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C113" s="0" t="str">
-        <f aca="false">C87</f>
+      <c r="G158" s="0" t="s">
+        <v>163</v>
+      </c>
+      <c r="H158" s="0" t="s">
+        <v>164</v>
+      </c>
+      <c r="J158" s="27" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="159" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C159" s="0" t="str">
+        <f aca="false">C133</f>
         <v>1PKE_0d</v>
       </c>
-      <c r="D113" s="0" t="n">
+      <c r="D159" s="0" t="n">
         <f aca="false">_xlfn.CEILING.MATH(G5*8/64)</f>
         <v>89</v>
       </c>
-      <c r="E113" s="0" t="n">
+      <c r="E159" s="0" t="n">
         <f aca="false">_xlfn.CEILING.MATH(I4*8/64)</f>
         <v>4</v>
       </c>
-      <c r="F113" s="0" t="n">
+      <c r="F159" s="0" t="n">
         <f aca="false">L18</f>
         <v>1579</v>
       </c>
-      <c r="G113" s="0" t="e">
+      <c r="G159" s="0" t="e">
         <f aca="false">I64</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="H113" s="0" t="n">
+      <c r="H159" s="0" t="n">
         <f aca="false">I17+E17</f>
         <v>8</v>
       </c>
-      <c r="I113" s="0" t="s">
+      <c r="I159" s="0" t="s">
         <v>47</v>
       </c>
-      <c r="J113" s="0" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="114" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C114" s="0" t="str">
-        <f aca="false">C88</f>
+      <c r="J159" s="0" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="160" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C160" s="0" t="str">
+        <f aca="false">C134</f>
         <v>3PKE_0d</v>
       </c>
-      <c r="D114" s="0" t="n">
+      <c r="D160" s="0" t="n">
         <f aca="false">_xlfn.CEILING.MATH(G6*8/64)</f>
         <v>129</v>
       </c>
-      <c r="E114" s="0" t="n">
+      <c r="E160" s="0" t="n">
         <f aca="false">_xlfn.CEILING.MATH(I5*8/64)</f>
         <v>95</v>
       </c>
-      <c r="F114" s="0" t="n">
+      <c r="F160" s="0" t="n">
         <f aca="false">L19</f>
         <v>2043</v>
       </c>
-      <c r="G114" s="0" t="e">
+      <c r="G160" s="0" t="e">
         <f aca="false">I65</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="H114" s="0" t="n">
+      <c r="H160" s="0" t="n">
         <f aca="false">I18+E18</f>
         <v>12</v>
       </c>
-      <c r="I114" s="0" t="n">
-        <v>24</v>
-      </c>
-      <c r="J114" s="0" t="n">
+      <c r="I160" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="J160" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="K114" s="0" t="s">
+      <c r="K160" s="0" t="s">
         <v>60</v>
       </c>
-      <c r="L114" s="0" t="s">
+      <c r="L160" s="0" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="115" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C115" s="0" t="str">
-        <f aca="false">C89</f>
+    <row r="161" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C161" s="0" t="str">
+        <f aca="false">C135</f>
         <v>5PKE_0d</v>
       </c>
-      <c r="D115" s="0" t="n">
+      <c r="D161" s="0" t="n">
         <f aca="false">_xlfn.CEILING.MATH(G7*8/64)</f>
         <v>177</v>
       </c>
-      <c r="E115" s="0" t="n">
+      <c r="E161" s="0" t="n">
         <f aca="false">_xlfn.CEILING.MATH(I6*8/64)</f>
         <v>140</v>
       </c>
-      <c r="F115" s="0" t="n">
+      <c r="F161" s="0" t="n">
         <f aca="false">L20</f>
         <v>1179</v>
       </c>
-      <c r="G115" s="0" t="e">
+      <c r="G161" s="0" t="e">
         <f aca="false">I66</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="H115" s="0" t="n">
+      <c r="H161" s="0" t="n">
         <f aca="false">I19+E19</f>
         <v>16</v>
       </c>
-      <c r="I115" s="0" t="n">
-        <v>24</v>
-      </c>
-      <c r="J115" s="0" t="n">
+      <c r="I161" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="J161" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="K115" s="0" t="n">
+      <c r="K161" s="0" t="n">
         <f aca="false">_xlfn.CEILING.MATH(B2*C2/1088)*24</f>
         <v>168</v>
       </c>
-      <c r="L115" s="0" t="n">
+      <c r="L161" s="0" t="n">
         <f aca="false">_xlfn.CEILING.MATH(B2*2/64)</f>
         <v>20</v>
       </c>
-      <c r="M115" s="0" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="116" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C116" s="0" t="str">
-        <f aca="false">C90</f>
+      <c r="M161" s="0" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="162" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C162" s="0" t="str">
+        <f aca="false">C136</f>
         <v>1KEM_5d</v>
       </c>
-      <c r="D116" s="0" t="n">
+      <c r="D162" s="0" t="n">
         <f aca="false">_xlfn.CEILING.MATH(G8*8/64)</f>
         <v>2</v>
       </c>
-      <c r="E116" s="0" t="n">
+      <c r="E162" s="0" t="n">
         <f aca="false">_xlfn.CEILING.MATH(I7*8/64)</f>
         <v>191</v>
       </c>
-      <c r="F116" s="0" t="n">
+      <c r="F162" s="0" t="n">
         <f aca="false">L21</f>
         <v>1711</v>
       </c>
-      <c r="G116" s="0" t="e">
+      <c r="G162" s="0" t="e">
         <f aca="false">I67</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="H116" s="0" t="n">
+      <c r="H162" s="0" t="n">
         <f aca="false">I20+E20</f>
         <v>8</v>
       </c>
-      <c r="I116" s="0" t="n">
-        <v>24</v>
-      </c>
-      <c r="J116" s="0" t="n">
+      <c r="I162" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="J162" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="K116" s="0" t="n">
+      <c r="K162" s="0" t="n">
         <f aca="false">_xlfn.CEILING.MATH(B3*C3/1088)*24</f>
         <v>240</v>
       </c>
-      <c r="L116" s="0" t="n">
+      <c r="L162" s="0" t="n">
         <f aca="false">_xlfn.CEILING.MATH(B3*2/64)</f>
         <v>25</v>
       </c>
-      <c r="M116" s="0" t="n">
-        <f aca="false">L115</f>
+      <c r="M162" s="0" t="n">
+        <f aca="false">L161</f>
         <v>20</v>
       </c>
-      <c r="N116" s="0" t="s">
+      <c r="N162" s="0" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="117" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C117" s="0" t="str">
-        <f aca="false">C91</f>
+    <row r="163" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C163" s="0" t="str">
+        <f aca="false">C137</f>
         <v>3KEM_5d</v>
       </c>
-      <c r="D117" s="0" t="n">
+      <c r="D163" s="0" t="n">
         <f aca="false">_xlfn.CEILING.MATH(G9*8/64)</f>
         <v>3</v>
       </c>
-      <c r="E117" s="0" t="n">
+      <c r="E163" s="0" t="n">
         <f aca="false">_xlfn.CEILING.MATH(I8*8/64)</f>
         <v>2</v>
       </c>
-      <c r="F117" s="0" t="n">
+      <c r="F163" s="0" t="n">
         <f aca="false">L22</f>
         <v>2347</v>
       </c>
-      <c r="G117" s="0" t="e">
+      <c r="G163" s="0" t="e">
         <f aca="false">I68</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="H117" s="0" t="n">
+      <c r="H163" s="0" t="n">
         <f aca="false">I21+E21</f>
         <v>15</v>
       </c>
-      <c r="I117" s="0" t="n">
-        <v>24</v>
-      </c>
-      <c r="J117" s="0" t="n">
+      <c r="I163" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="J163" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="K117" s="0" t="n">
+      <c r="K163" s="0" t="n">
         <f aca="false">_xlfn.CEILING.MATH(B4*C4/1088)*24</f>
         <v>336</v>
       </c>
-      <c r="L117" s="0" t="n">
+      <c r="L163" s="0" t="n">
         <f aca="false">_xlfn.CEILING.MATH(B4*2/64)</f>
         <v>32</v>
       </c>
-      <c r="M117" s="0" t="n">
-        <f aca="false">L116</f>
+      <c r="M163" s="0" t="n">
+        <f aca="false">L162</f>
         <v>25</v>
       </c>
-      <c r="N117" s="0" t="n">
+      <c r="N163" s="0" t="n">
         <f aca="false">K17</f>
         <v>2482</v>
       </c>
-      <c r="O117" s="0" t="s">
+      <c r="O163" s="0" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="118" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C118" s="0" t="str">
-        <f aca="false">C92</f>
+    <row r="164" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C164" s="0" t="str">
+        <f aca="false">C138</f>
         <v>5KEM_5d</v>
       </c>
-      <c r="D118" s="0" t="n">
+      <c r="D164" s="0" t="n">
         <f aca="false">_xlfn.CEILING.MATH(G10*8/64)</f>
         <v>4</v>
       </c>
-      <c r="E118" s="0" t="n">
+      <c r="E164" s="0" t="n">
         <f aca="false">_xlfn.CEILING.MATH(I9*8/64)</f>
         <v>3</v>
       </c>
-      <c r="F118" s="0" t="n">
+      <c r="F164" s="0" t="n">
         <f aca="false">L23</f>
         <v>987</v>
       </c>
-      <c r="G118" s="0" t="e">
+      <c r="G164" s="0" t="e">
         <f aca="false">I69</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="H118" s="0" t="n">
+      <c r="H164" s="0" t="n">
         <f aca="false">I22+E22</f>
         <v>20</v>
       </c>
-      <c r="I118" s="0" t="n">
-        <v>24</v>
-      </c>
-      <c r="J118" s="0" t="n">
+      <c r="I164" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="J164" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="K118" s="0" t="n">
+      <c r="K164" s="0" t="n">
         <f aca="false">_xlfn.CEILING.MATH(B5*C5/1088)*24</f>
         <v>192</v>
       </c>
-      <c r="L118" s="0" t="n">
+      <c r="L164" s="0" t="n">
         <f aca="false">_xlfn.CEILING.MATH(B5*2/64)</f>
         <v>19</v>
       </c>
-      <c r="M118" s="0" t="n">
-        <f aca="false">L117</f>
+      <c r="M164" s="0" t="n">
+        <f aca="false">L163</f>
         <v>32</v>
       </c>
-      <c r="N118" s="0" t="n">
+      <c r="N164" s="0" t="n">
         <f aca="false">K18</f>
         <v>3154</v>
       </c>
-      <c r="O118" s="0" t="n">
-        <v>24</v>
-      </c>
-      <c r="P118" s="0" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="119" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C119" s="0" t="str">
-        <f aca="false">C93</f>
+      <c r="O164" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="P164" s="0" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="165" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C165" s="0" t="str">
+        <f aca="false">C139</f>
         <v>1PKE_5d</v>
       </c>
-      <c r="D119" s="0" t="n">
+      <c r="D165" s="0" t="n">
         <f aca="false">_xlfn.CEILING.MATH(G11*8/64)</f>
         <v>62</v>
       </c>
-      <c r="E119" s="0" t="n">
+      <c r="E165" s="0" t="n">
         <f aca="false">_xlfn.CEILING.MATH(I10*8/64)</f>
         <v>4</v>
       </c>
-      <c r="F119" s="0" t="n">
+      <c r="F165" s="0" t="n">
         <f aca="false">L24</f>
         <v>1519</v>
       </c>
-      <c r="G119" s="0" t="n">
+      <c r="G165" s="0" t="n">
         <f aca="false">I70</f>
         <v>24</v>
       </c>
-      <c r="H119" s="0" t="n">
+      <c r="H165" s="0" t="n">
         <f aca="false">I23+E23</f>
         <v>30</v>
       </c>
-      <c r="I119" s="0" t="n">
-        <v>24</v>
-      </c>
-      <c r="J119" s="0" t="n">
+      <c r="I165" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="J165" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="K119" s="0" t="n">
+      <c r="K165" s="0" t="n">
         <f aca="false">_xlfn.CEILING.MATH(B6*C6/1088)*24</f>
         <v>240</v>
       </c>
-      <c r="L119" s="0" t="n">
+      <c r="L165" s="0" t="n">
         <f aca="false">_xlfn.CEILING.MATH(B6*2/64)</f>
         <v>27</v>
       </c>
-      <c r="M119" s="0" t="n">
-        <f aca="false">L118</f>
+      <c r="M165" s="0" t="n">
+        <f aca="false">L164</f>
         <v>19</v>
       </c>
-      <c r="N119" s="0" t="n">
+      <c r="N165" s="0" t="n">
         <f aca="false">K19</f>
         <v>4082</v>
       </c>
-      <c r="O119" s="0" t="n">
-        <v>24</v>
-      </c>
-      <c r="P119" s="0" t="n">
-        <v>24</v>
-      </c>
-      <c r="Q119" s="0" t="s">
-        <v>162</v>
-      </c>
-      <c r="R119" s="26" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="120" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C120" s="0" t="str">
-        <f aca="false">C94</f>
+      <c r="O165" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="P165" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="Q165" s="0" t="s">
+        <v>168</v>
+      </c>
+      <c r="R165" s="26" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="166" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C166" s="0" t="str">
+        <f aca="false">C140</f>
         <v>3PKE_5d</v>
       </c>
-      <c r="D120" s="0" t="n">
+      <c r="D166" s="0" t="n">
         <f aca="false">_xlfn.CEILING.MATH(G12*8/64)</f>
         <v>104</v>
       </c>
-      <c r="E120" s="0" t="n">
+      <c r="E166" s="0" t="n">
         <f aca="false">_xlfn.CEILING.MATH(I11*8/64)</f>
         <v>79</v>
       </c>
-      <c r="F120" s="0" t="n">
+      <c r="F166" s="0" t="n">
         <f aca="false">L25</f>
         <v>1887</v>
       </c>
-      <c r="G120" s="0" t="n">
+      <c r="G166" s="0" t="n">
         <f aca="false">I71</f>
         <v>30</v>
       </c>
-      <c r="H120" s="0" t="n">
+      <c r="H166" s="0" t="n">
         <f aca="false">I24+E24</f>
         <v>34</v>
       </c>
-      <c r="I120" s="0" t="n">
-        <v>24</v>
-      </c>
-      <c r="J120" s="0" t="n">
+      <c r="I166" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="J166" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="K120" s="0" t="n">
+      <c r="K166" s="0" t="n">
         <f aca="false">_xlfn.CEILING.MATH(B7*C7/1088)*24</f>
         <v>336</v>
       </c>
-      <c r="L120" s="0" t="n">
+      <c r="L166" s="0" t="n">
         <f aca="false">_xlfn.CEILING.MATH(B7*2/64)</f>
         <v>37</v>
       </c>
-      <c r="M120" s="0" t="n">
-        <f aca="false">L119</f>
+      <c r="M166" s="0" t="n">
+        <f aca="false">L165</f>
         <v>27</v>
       </c>
-      <c r="N120" s="0" t="n">
+      <c r="N166" s="0" t="n">
         <f aca="false">K20</f>
         <v>2354</v>
       </c>
-      <c r="O120" s="0" t="n">
-        <v>24</v>
-      </c>
-      <c r="P120" s="0" t="n">
-        <v>24</v>
-      </c>
-      <c r="Q120" s="0" t="n">
+      <c r="O166" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="P166" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="Q166" s="0" t="n">
         <f aca="false">J2*8/64</f>
         <v>2</v>
       </c>
-      <c r="R120" s="0" t="n">
-        <f aca="false">Q120+P119+O118+N117+M116+K115+J114+H113+F112+E111+D110</f>
+      <c r="R166" s="0" t="n">
+        <f aca="false">Q166+P165+O164+N163+M162+K161+J160+H159+F158+E157+D156</f>
         <v>3975</v>
       </c>
     </row>
-    <row r="121" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C121" s="0" t="str">
-        <f aca="false">C95</f>
+    <row r="167" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C167" s="0" t="str">
+        <f aca="false">C141</f>
         <v>5PKE_5d</v>
       </c>
-      <c r="D121" s="0" t="n">
+      <c r="D167" s="0" t="n">
         <f aca="false">_xlfn.CEILING.MATH(G13*8/64)</f>
         <v>131</v>
       </c>
-      <c r="E121" s="0" t="n">
+      <c r="E167" s="0" t="n">
         <f aca="false">_xlfn.CEILING.MATH(I12*8/64)</f>
         <v>119</v>
       </c>
-      <c r="F121" s="0" t="n">
+      <c r="F167" s="0" t="n">
         <f aca="false">L26</f>
         <v>1023</v>
       </c>
-      <c r="G121" s="0" t="n">
+      <c r="G167" s="0" t="n">
         <f aca="false">I72</f>
         <v>32</v>
       </c>
-      <c r="H121" s="0" t="n">
+      <c r="H167" s="0" t="n">
         <f aca="false">I25+E25</f>
         <v>38</v>
       </c>
-      <c r="I121" s="0" t="n">
-        <v>24</v>
-      </c>
-      <c r="J121" s="0" t="n">
+      <c r="I167" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="J167" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="K121" s="0" t="n">
+      <c r="K167" s="0" t="n">
         <f aca="false">_xlfn.CEILING.MATH(B8*C8/1088)*24</f>
         <v>120</v>
       </c>
-      <c r="L121" s="0" t="n">
+      <c r="L167" s="0" t="n">
         <f aca="false">_xlfn.CEILING.MATH(B8*2/64)</f>
         <v>16</v>
       </c>
-      <c r="M121" s="0" t="n">
-        <f aca="false">L120</f>
+      <c r="M167" s="0" t="n">
+        <f aca="false">L166</f>
         <v>37</v>
       </c>
-      <c r="N121" s="0" t="n">
+      <c r="N167" s="0" t="n">
         <f aca="false">K21</f>
         <v>3418</v>
       </c>
-      <c r="O121" s="0" t="n">
-        <v>24</v>
-      </c>
-      <c r="P121" s="0" t="n">
-        <v>24</v>
-      </c>
-      <c r="Q121" s="0" t="n">
+      <c r="O167" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="P167" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="Q167" s="0" t="n">
         <f aca="false">J3*8/64</f>
         <v>3</v>
       </c>
-      <c r="R121" s="0" t="n">
-        <f aca="false">Q121+P120+O119+N118+M117+K116+J115+H114+F113+E112+D111</f>
+      <c r="R167" s="0" t="n">
+        <f aca="false">Q167+P166+O165+N164+M163+K162+J161+H160+F159+E158+D157</f>
         <v>5067</v>
       </c>
     </row>
-    <row r="122" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E122" s="0" t="n">
+    <row r="168" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E168" s="0" t="n">
         <f aca="false">_xlfn.CEILING.MATH(I13*8/64)</f>
         <v>163</v>
       </c>
-      <c r="F122" s="0" t="n">
+      <c r="F168" s="0" t="n">
         <f aca="false">L27</f>
         <v>1519</v>
       </c>
-      <c r="G122" s="0" t="n">
+      <c r="G168" s="0" t="n">
         <f aca="false">I73</f>
         <v>24</v>
       </c>
-      <c r="H122" s="0" t="n">
+      <c r="H168" s="0" t="n">
         <f aca="false">I26+E26</f>
         <v>32</v>
       </c>
-      <c r="I122" s="0" t="n">
-        <v>24</v>
-      </c>
-      <c r="J122" s="0" t="n">
+      <c r="I168" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="J168" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="K122" s="0" t="n">
+      <c r="K168" s="0" t="n">
         <f aca="false">_xlfn.CEILING.MATH(B9*C9/1088)*24</f>
         <v>216</v>
       </c>
-      <c r="L122" s="0" t="n">
+      <c r="L168" s="0" t="n">
         <f aca="false">_xlfn.CEILING.MATH(B9*2/64)</f>
         <v>24</v>
       </c>
-      <c r="M122" s="0" t="n">
-        <f aca="false">L121</f>
+      <c r="M168" s="0" t="n">
+        <f aca="false">L167</f>
         <v>16</v>
       </c>
-      <c r="N122" s="0" t="n">
+      <c r="N168" s="0" t="n">
         <f aca="false">K22</f>
         <v>4690</v>
       </c>
-      <c r="O122" s="0" t="n">
-        <v>24</v>
-      </c>
-      <c r="P122" s="0" t="n">
-        <v>24</v>
-      </c>
-      <c r="Q122" s="0" t="n">
+      <c r="O168" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="P168" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="Q168" s="0" t="n">
         <f aca="false">J4*8/64</f>
         <v>4</v>
       </c>
-      <c r="R122" s="0" t="n">
-        <f aca="false">Q122+P121+O120+N119+M118+K117+J116+H115+F114+E113+D112</f>
+      <c r="R168" s="0" t="n">
+        <f aca="false">Q168+P167+O166+N165+M164+K163+J162+H161+F160+E159+D158</f>
         <v>6569</v>
       </c>
     </row>
-    <row r="123" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F123" s="0" t="n">
+    <row r="169" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F169" s="0" t="n">
         <f aca="false">L28</f>
         <v>1899</v>
       </c>
-      <c r="G123" s="0" t="n">
+      <c r="G169" s="0" t="n">
         <f aca="false">I74</f>
         <v>30</v>
       </c>
-      <c r="H123" s="0" t="n">
+      <c r="H169" s="0" t="n">
         <f aca="false">I27+E27</f>
         <v>37</v>
       </c>
-      <c r="I123" s="0" t="n">
-        <v>24</v>
-      </c>
-      <c r="J123" s="0" t="n">
+      <c r="I169" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="J169" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="K123" s="0" t="n">
+      <c r="K169" s="0" t="n">
         <f aca="false">_xlfn.CEILING.MATH(B10*C10/1088)*24</f>
         <v>264</v>
       </c>
-      <c r="L123" s="0" t="n">
+      <c r="L169" s="0" t="n">
         <f aca="false">_xlfn.CEILING.MATH(B10*2/64)</f>
         <v>30</v>
       </c>
-      <c r="M123" s="0" t="n">
-        <f aca="false">L122</f>
-        <v>24</v>
-      </c>
-      <c r="N123" s="0" t="n">
+      <c r="M169" s="0" t="n">
+        <f aca="false">L168</f>
+        <v>24</v>
+      </c>
+      <c r="N169" s="0" t="n">
         <f aca="false">K23</f>
         <v>1970</v>
       </c>
-      <c r="O123" s="0" t="n">
-        <v>24</v>
-      </c>
-      <c r="P123" s="0" t="n">
-        <v>24</v>
-      </c>
-      <c r="Q123" s="0" t="n">
+      <c r="O169" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="P169" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="Q169" s="0" t="n">
         <f aca="false">J5*8/64</f>
         <v>2</v>
       </c>
-      <c r="R123" s="0" t="n">
-        <f aca="false">Q123+P122+O121+N120+M119+K118+J117+H116+F115+E114+D113</f>
+      <c r="R169" s="0" t="n">
+        <f aca="false">Q169+P168+O167+N166+M165+K164+J163+H162+F161+E160+D159</f>
         <v>3986</v>
       </c>
     </row>
-    <row r="124" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G124" s="0" t="n">
+    <row r="170" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G170" s="0" t="n">
         <f aca="false">I75</f>
         <v>32</v>
       </c>
-      <c r="H124" s="0" t="n">
+      <c r="H170" s="0" t="n">
         <f aca="false">I28+E28</f>
         <v>50</v>
       </c>
-      <c r="I124" s="0" t="n">
-        <v>24</v>
-      </c>
-      <c r="J124" s="0" t="n">
+      <c r="I170" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="J170" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="K124" s="0" t="n">
+      <c r="K170" s="0" t="n">
         <f aca="false">_xlfn.CEILING.MATH(B11*C11/1088)*24</f>
         <v>120</v>
       </c>
-      <c r="L124" s="0" t="n">
+      <c r="L170" s="0" t="n">
         <f aca="false">_xlfn.CEILING.MATH(B11*2/64)</f>
         <v>16</v>
       </c>
-      <c r="M124" s="0" t="n">
-        <f aca="false">L123</f>
+      <c r="M170" s="0" t="n">
+        <f aca="false">L169</f>
         <v>30</v>
       </c>
-      <c r="N124" s="0" t="n">
+      <c r="N170" s="0" t="n">
         <f aca="false">K24</f>
         <v>3034</v>
       </c>
-      <c r="O124" s="0" t="n">
-        <v>24</v>
-      </c>
-      <c r="P124" s="0" t="n">
-        <v>24</v>
-      </c>
-      <c r="Q124" s="0" t="n">
+      <c r="O170" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="P170" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="Q170" s="0" t="n">
         <f aca="false">J6*8/64</f>
         <v>3</v>
       </c>
-      <c r="R124" s="0" t="n">
-        <f aca="false">Q124+P123+O122+N121+M120+K119+J118+H117+F116+E115+D114</f>
+      <c r="R170" s="0" t="n">
+        <f aca="false">Q170+P169+O168+N167+M166+K165+J164+H163+F162+E161+D160</f>
         <v>5731</v>
       </c>
     </row>
-    <row r="125" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I125" s="0" t="n">
-        <v>24</v>
-      </c>
-      <c r="J125" s="0" t="n">
+    <row r="171" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I171" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="J171" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="K125" s="0" t="n">
+      <c r="K171" s="0" t="n">
         <f aca="false">_xlfn.CEILING.MATH(B12*C12/1088)*24</f>
         <v>216</v>
       </c>
-      <c r="L125" s="0" t="n">
+      <c r="L171" s="0" t="n">
         <f aca="false">_xlfn.CEILING.MATH(B12*2/64)</f>
         <v>24</v>
       </c>
-      <c r="M125" s="0" t="n">
-        <f aca="false">L124</f>
+      <c r="M171" s="0" t="n">
+        <f aca="false">L170</f>
         <v>16</v>
       </c>
-      <c r="N125" s="0" t="n">
+      <c r="N171" s="0" t="n">
         <f aca="false">K25</f>
         <v>3770</v>
       </c>
-      <c r="O125" s="0" t="n">
-        <v>24</v>
-      </c>
-      <c r="P125" s="0" t="n">
-        <v>24</v>
-      </c>
-      <c r="Q125" s="0" t="n">
+      <c r="O171" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="P171" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="Q171" s="0" t="n">
         <f aca="false">J7*8/64</f>
         <v>4</v>
       </c>
-      <c r="R125" s="0" t="n">
-        <f aca="false">Q125+P124+O123+N122+M121+K120+J119+H118+F117+E116+D115</f>
+      <c r="R171" s="0" t="n">
+        <f aca="false">Q171+P170+O169+N168+M167+K166+J165+H164+F163+E162+D161</f>
         <v>7850</v>
       </c>
     </row>
-    <row r="126" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K126" s="0" t="n">
+    <row r="172" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K172" s="0" t="n">
         <f aca="false">_xlfn.CEILING.MATH(B13*C13/1088)*24</f>
         <v>240</v>
       </c>
-      <c r="L126" s="0" t="n">
+      <c r="L172" s="0" t="n">
         <f aca="false">_xlfn.CEILING.MATH(B13*2/64)</f>
         <v>30</v>
       </c>
-      <c r="M126" s="0" t="n">
-        <f aca="false">L125</f>
-        <v>24</v>
-      </c>
-      <c r="N126" s="0" t="n">
+      <c r="M172" s="0" t="n">
+        <f aca="false">L171</f>
+        <v>24</v>
+      </c>
+      <c r="N172" s="0" t="n">
         <f aca="false">K26</f>
         <v>2042</v>
       </c>
-      <c r="O126" s="0" t="n">
-        <v>24</v>
-      </c>
-      <c r="P126" s="0" t="n">
-        <v>24</v>
-      </c>
-      <c r="Q126" s="0" t="n">
+      <c r="O172" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="P172" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="Q172" s="0" t="n">
         <f aca="false">J8*8/64</f>
         <v>2</v>
       </c>
-      <c r="R126" s="0" t="n">
-        <f aca="false">Q126+P125+O124+N123+M122+K121+J120+H119+F118+E117+D116+G119</f>
+      <c r="R172" s="0" t="n">
+        <f aca="false">Q172+P171+O170+N169+M168+K167+J166+H165+F164+E163+D162+G165</f>
         <v>3201</v>
       </c>
     </row>
-    <row r="127" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="M127" s="0" t="n">
-        <f aca="false">L126</f>
+    <row r="173" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M173" s="0" t="n">
+        <f aca="false">L172</f>
         <v>30</v>
       </c>
-      <c r="N127" s="0" t="n">
+      <c r="N173" s="0" t="n">
         <f aca="false">K27</f>
         <v>3034</v>
       </c>
-      <c r="O127" s="0" t="n">
-        <v>24</v>
-      </c>
-      <c r="P127" s="0" t="n">
-        <v>24</v>
-      </c>
-      <c r="Q127" s="0" t="n">
+      <c r="O173" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="P173" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="Q173" s="0" t="n">
         <f aca="false">J9*8/64</f>
         <v>3</v>
       </c>
-      <c r="R127" s="0" t="n">
-        <f aca="false">Q127+P126+O125+N124+M123+K122+J121+H120+F119+E118+D117+G120</f>
+      <c r="R173" s="0" t="n">
+        <f aca="false">Q173+P172+O171+N170+M169+K168+J167+H166+F165+E164+D163+G166</f>
         <v>4914</v>
       </c>
     </row>
-    <row r="128" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="N128" s="0" t="n">
+    <row r="174" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="N174" s="0" t="n">
         <f aca="false">K28</f>
         <v>3794</v>
       </c>
-      <c r="O128" s="0" t="n">
-        <v>24</v>
-      </c>
-      <c r="P128" s="0" t="n">
-        <v>24</v>
-      </c>
-      <c r="Q128" s="0" t="n">
+      <c r="O174" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="P174" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="Q174" s="0" t="n">
         <f aca="false">J10*8/64</f>
         <v>4</v>
       </c>
-      <c r="R128" s="0" t="n">
-        <f aca="false">Q128+P127+O126+N125+M124+K123+J122+H121+F120+E119+D118+G121</f>
+      <c r="R174" s="0" t="n">
+        <f aca="false">Q174+P173+O172+N171+M170+K169+J168+H167+F166+E165+D164+G167</f>
         <v>6081</v>
       </c>
     </row>
-    <row r="129" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O129" s="0" t="n">
-        <v>24</v>
-      </c>
-      <c r="P129" s="0" t="n">
-        <v>24</v>
-      </c>
-      <c r="Q129" s="0" t="n">
+    <row r="175" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="O175" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="P175" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="Q175" s="0" t="n">
         <f aca="false">J11*8/64</f>
         <v>2</v>
       </c>
-      <c r="R129" s="0" t="n">
-        <f aca="false">Q129+P128+O127+N126+M125+K124+J123+H122+F121+E120+D119+G122</f>
+      <c r="R175" s="0" t="n">
+        <f aca="false">Q175+P174+O173+N172+M171+K170+J169+H168+F167+E166+D165+G168</f>
         <v>3448</v>
       </c>
     </row>
-    <row r="130" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="P130" s="0" t="n">
-        <v>24</v>
-      </c>
-      <c r="Q130" s="0" t="n">
+    <row r="176" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="P176" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="Q176" s="0" t="n">
         <f aca="false">J12*8/64</f>
         <v>3</v>
       </c>
-      <c r="R130" s="0" t="n">
-        <f aca="false">Q130+P129+O128+N127+M126+K125+J124+H123+F122+E121+D120+G123</f>
+      <c r="R176" s="0" t="n">
+        <f aca="false">Q176+P175+O174+N173+M172+K171+J170+H169+F168+E167+D166+G169</f>
         <v>5134</v>
       </c>
     </row>
-    <row r="131" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Q131" s="0" t="n">
+    <row r="177" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="Q177" s="0" t="n">
         <f aca="false">J13*8/64</f>
         <v>4</v>
       </c>
-      <c r="R131" s="0" t="n">
-        <f aca="false">Q131+P130+O129+N128+M127+K126+J125+H124+F123+E122+D121+G124</f>
+      <c r="R177" s="0" t="n">
+        <f aca="false">Q177+P176+O175+N174+M173+K172+J171+H170+F169+E168+D167+G170</f>
         <v>6391</v>
       </c>
     </row>
-    <row r="132" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="178" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>